<commit_message>
work on search chart in screen
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="План" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Модуль для торговли через эмуляцию нажатий мыши и клавиш</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Изучить возможности работы с графиками с помощью OpenCV</t>
+  </si>
+  <si>
+    <t>Оптимизировать с помощью серых цветов</t>
   </si>
 </sst>
 </file>
@@ -884,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B213"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +956,9 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2005,7 +2010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T220"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2024,7 +2029,7 @@
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E1" s="12">
         <f ca="1">NOW()</f>
-        <v>45435.038388194444</v>
+        <v>45435.631103472224</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -2113,7 +2118,7 @@
       <c r="E4" s="10"/>
       <c r="F4" s="4">
         <f ca="1">ROUND(IF(E4,E4-D4,$E$1-D4),0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
work on the quick_test
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Модуль для торговли через эмуляцию нажатий мыши и клавиш</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Покупает в нижней части графика, продает в верхней</t>
   </si>
   <si>
-    <t>Тестируется</t>
-  </si>
-  <si>
     <t>Бот хорошо работает, когда на графике боковик, но может сильно провиснуть, когда инструмент безоткатно падает. В целом бот может приносить прибыль, если периодически подбирать графики</t>
   </si>
   <si>
@@ -137,11 +134,29 @@
   <si>
     <t>Оптимизировать с помощью серых цветов</t>
   </si>
+  <si>
+    <t>Трендер-1</t>
+  </si>
+  <si>
+    <t>Попытка торговли по тренду</t>
+  </si>
+  <si>
+    <t>Бот оказался провальным. Он не спас от проливов рынка, как ожидалось</t>
+  </si>
+  <si>
+    <t>Создать консультанта по торговле</t>
+  </si>
+  <si>
+    <t>Рассмотреть дебаггинг декомпилированной версии</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -224,6 +239,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -528,7 +546,7 @@
   <dimension ref="A2:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +906,7 @@
   <dimension ref="A2:B213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,16 +958,16 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>37</v>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>38</v>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -957,20 +975,24 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2011,7 +2033,7 @@
   <dimension ref="A1:T220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2051,7 @@
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E1" s="12">
         <f ca="1">NOW()</f>
-        <v>45435.631103472224</v>
+        <v>45442.74202986111</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -2087,7 +2109,7 @@
       <c r="H3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="14">
         <v>2.9</v>
       </c>
       <c r="J3" s="8"/>
@@ -2115,18 +2137,20 @@
       <c r="D4" s="10">
         <v>45433</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10">
+        <v>45435</v>
+      </c>
       <c r="F4" s="4">
-        <f ca="1">ROUND(IF(E4,E4-D4,$E$1-D4),0)</f>
-        <v>3</v>
-      </c>
-      <c r="G4" s="8" t="s">
+        <f>ROUND(IF(E4,E4-D4,$E$1-D4),0)</f>
+        <v>2</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="4">
+      <c r="I4" s="14">
         <v>3.6</v>
       </c>
       <c r="J4" s="8"/>
@@ -2141,16 +2165,35 @@
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="10">
+        <v>45442</v>
+      </c>
+      <c r="E5" s="10">
+        <v>45442</v>
+      </c>
+      <c r="F5" s="4">
+        <f>ROUND(IF(E5,E5-D5,$E$1-D5),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="14">
+        <v>3</v>
+      </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
@@ -2173,6 +2216,7 @@
       <c r="E6" s="4"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
@@ -2195,6 +2239,7 @@
       <c r="E7" s="4"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
+      <c r="I7" s="14"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
@@ -2217,6 +2262,7 @@
       <c r="E8" s="4"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
+      <c r="I8" s="14"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
@@ -2239,6 +2285,7 @@
       <c r="E9" s="4"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
+      <c r="I9" s="14"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -2261,6 +2308,7 @@
       <c r="E10" s="4"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -2283,6 +2331,7 @@
       <c r="E11" s="4"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -2305,6 +2354,7 @@
       <c r="E12" s="4"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -2327,6 +2377,7 @@
       <c r="E13" s="4"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
+      <c r="I13" s="14"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
@@ -2349,6 +2400,7 @@
       <c r="E14" s="4"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -2371,6 +2423,7 @@
       <c r="E15" s="4"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
@@ -2393,6 +2446,7 @@
       <c r="E16" s="4"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
@@ -2415,6 +2469,7 @@
       <c r="E17" s="4"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
@@ -2437,6 +2492,7 @@
       <c r="E18" s="4"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
+      <c r="I18" s="14"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
@@ -2459,6 +2515,7 @@
       <c r="E19" s="4"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
+      <c r="I19" s="14"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
@@ -2481,6 +2538,7 @@
       <c r="E20" s="4"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
@@ -2503,6 +2561,7 @@
       <c r="E21" s="4"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
+      <c r="I21" s="14"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
@@ -2525,6 +2584,7 @@
       <c r="E22" s="4"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
+      <c r="I22" s="14"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
@@ -2547,6 +2607,7 @@
       <c r="E23" s="4"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
+      <c r="I23" s="14"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
@@ -2569,6 +2630,7 @@
       <c r="E24" s="4"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
+      <c r="I24" s="14"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
@@ -2591,6 +2653,7 @@
       <c r="E25" s="4"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
+      <c r="I25" s="14"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
@@ -2613,6 +2676,7 @@
       <c r="E26" s="4"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
+      <c r="I26" s="14"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -2635,6 +2699,7 @@
       <c r="E27" s="4"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
+      <c r="I27" s="14"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
@@ -2657,6 +2722,7 @@
       <c r="E28" s="4"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
+      <c r="I28" s="14"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
@@ -2679,6 +2745,7 @@
       <c r="E29" s="4"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
+      <c r="I29" s="14"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
@@ -2701,6 +2768,7 @@
       <c r="E30" s="4"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
+      <c r="I30" s="14"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
@@ -2723,6 +2791,7 @@
       <c r="E31" s="4"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
+      <c r="I31" s="14"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
@@ -2745,6 +2814,7 @@
       <c r="E32" s="4"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
+      <c r="I32" s="14"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>

</xml_diff>

<commit_message>
add indicators SMA and BB
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="План" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t>Модуль для торговли через эмуляцию нажатий мыши и клавиш</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>Абстрактный бот</t>
+  </si>
+  <si>
+    <t>Поколение</t>
+  </si>
+  <si>
+    <t>МультиТрендер-1</t>
+  </si>
+  <si>
+    <t>Торговля по тренду разных таймфремов</t>
+  </si>
+  <si>
+    <t>Абстракт-1</t>
   </si>
 </sst>
 </file>
@@ -261,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -298,6 +310,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2087,31 +2105,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T220"/>
+  <dimension ref="A1:U221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="38.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="4"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="31" style="15" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E1" s="12">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F1" s="12">
         <f ca="1">NOW()</f>
-        <v>45494.866448726854</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45497.62455763889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2119,98 +2138,89 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="10">
-        <v>45419</v>
-      </c>
-      <c r="E3" s="10">
-        <v>45420</v>
-      </c>
-      <c r="F3" s="4">
-        <f>ROUND(IF(E3,E3-D3,$E$1-D3),0)</f>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="D3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="16">
+        <v>45401</v>
+      </c>
+      <c r="F3" s="16">
+        <v>45494</v>
+      </c>
+      <c r="G3" s="4">
+        <f>ROUND(IF(F3,F3-E3,$F$1-E3),0)</f>
+        <v>93</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-    </row>
-    <row r="4" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="10">
-        <v>45433</v>
+        <v>22</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="E4" s="10">
-        <v>45435</v>
-      </c>
-      <c r="F4" s="4">
-        <f>ROUND(IF(E4,E4-D4,$E$1-D4),0)</f>
-        <v>2</v>
-      </c>
-      <c r="G4" s="11" t="s">
+        <v>45419</v>
+      </c>
+      <c r="F4" s="10">
+        <v>45420</v>
+      </c>
+      <c r="G4" s="4">
+        <f>ROUND(IF(F4,F4-E4,$F$1-E4),0)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="14">
-        <v>3.6</v>
-      </c>
-      <c r="J4" s="8"/>
+      <c r="I4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="14">
+        <v>2.9</v>
+      </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
@@ -2221,37 +2231,40 @@
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
-    </row>
-    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U4" s="8"/>
+    </row>
+    <row r="5" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="10">
-        <v>45442</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="E5" s="10">
-        <v>45442</v>
-      </c>
-      <c r="F5" s="4">
-        <f>ROUND(IF(E5,E5-D5,$E$1-D5),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="11" t="s">
+        <v>45433</v>
+      </c>
+      <c r="F5" s="10">
+        <v>45435</v>
+      </c>
+      <c r="G5" s="4">
+        <f>ROUND(IF(F5,F5-E5,$F$1-E5),0)</f>
+        <v>2</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="14">
-        <v>3</v>
-      </c>
-      <c r="J5" s="8"/>
+      <c r="I5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="14">
+        <v>3.6</v>
+      </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
@@ -2262,37 +2275,40 @@
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
-    </row>
-    <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U5" s="8"/>
+    </row>
+    <row r="6" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="10">
-        <v>45457</v>
+        <v>38</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="E6" s="10">
-        <v>45480</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" ref="F6:F12" si="0">ROUND(IF(E6,E6-D6,$E$1-D6),0)</f>
-        <v>23</v>
-      </c>
-      <c r="G6" s="11" t="s">
+        <v>45442</v>
+      </c>
+      <c r="F6" s="10">
+        <v>45442</v>
+      </c>
+      <c r="G6" s="4">
+        <f>ROUND(IF(F6,F6-E6,$F$1-E6),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="14">
-        <v>3.9</v>
-      </c>
-      <c r="J6" s="8"/>
+      <c r="I6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="14">
+        <v>3</v>
+      </c>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -2303,37 +2319,40 @@
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
-    </row>
-    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U6" s="8"/>
+    </row>
+    <row r="7" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="10">
-        <v>45475</v>
+        <v>43</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="E7" s="10">
-        <v>45475</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="11" t="s">
+        <v>45457</v>
+      </c>
+      <c r="F7" s="10">
+        <v>45480</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" ref="G7:G13" si="0">ROUND(IF(F7,F7-E7,$F$1-E7),0)</f>
+        <v>23</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="14">
-        <v>1.3</v>
-      </c>
-      <c r="J7" s="8"/>
+      <c r="I7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="14">
+        <v>3.9</v>
+      </c>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -2344,37 +2363,40 @@
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="8"/>
+    </row>
+    <row r="8" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="10">
-        <v>45477</v>
+        <v>46</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="E8" s="10">
-        <v>45480</v>
-      </c>
-      <c r="F8" s="4">
+        <v>45475</v>
+      </c>
+      <c r="F8" s="10">
+        <v>45475</v>
+      </c>
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G8" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="14">
-        <v>4</v>
-      </c>
-      <c r="J8" s="8"/>
+      <c r="I8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="14">
+        <v>1.3</v>
+      </c>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -2385,35 +2407,40 @@
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="8"/>
+    </row>
+    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="10">
+        <v>49</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="10">
         <v>45477</v>
       </c>
-      <c r="E9" s="10">
-        <v>45481</v>
-      </c>
-      <c r="F9" s="4">
+      <c r="F9" s="10">
+        <v>45480</v>
+      </c>
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="14">
         <v>4</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -2424,37 +2451,38 @@
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="8"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="10">
+        <v>50</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="10">
         <v>45477</v>
       </c>
-      <c r="E10" s="10">
-        <v>45480</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="F10" s="10">
+        <v>45481</v>
+      </c>
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="14">
-        <v>3.2</v>
-      </c>
-      <c r="J10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="14">
+        <v>4.0999999999999996</v>
+      </c>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -2465,35 +2493,40 @@
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="8"/>
+    </row>
+    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="10">
+        <v>51</v>
+      </c>
+      <c r="C11" s="8">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="10">
+        <v>45477</v>
+      </c>
+      <c r="F11" s="10">
         <v>45480</v>
       </c>
-      <c r="E11" s="10">
-        <v>45481</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J11" s="8"/>
+      <c r="I11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="14">
+        <v>3.2</v>
+      </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
@@ -2504,29 +2537,38 @@
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="8"/>
+    </row>
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="10">
-        <v>45494</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4">
-        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="10">
+        <v>45480</v>
+      </c>
+      <c r="F12" s="10">
+        <v>45481</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="8"/>
+      <c r="H12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="14">
+        <v>4.0999999999999996</v>
+      </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
@@ -2537,19 +2579,32 @@
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="8"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="G13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="10">
+        <v>45494</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
       <c r="H13" s="8"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
@@ -2560,19 +2615,26 @@
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="8"/>
+    </row>
+    <row r="14" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="E14" s="4"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="4"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="8"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -2583,19 +2645,20 @@
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="8"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="4"/>
-      <c r="G15" s="8"/>
+      <c r="F15" s="4"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="8"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -2606,19 +2669,20 @@
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" s="8"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="4"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="4"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="8"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="14"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -2629,19 +2693,20 @@
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16" s="8"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="4"/>
-      <c r="G17" s="8"/>
+      <c r="F17" s="4"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -2652,19 +2717,20 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="8"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="4"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="4"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="8"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="14"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -2675,19 +2741,20 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="8"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="4"/>
-      <c r="G19" s="8"/>
+      <c r="F19" s="4"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="8"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="14"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -2698,19 +2765,20 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="8"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="4"/>
-      <c r="G20" s="8"/>
+      <c r="F20" s="4"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="8"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="14"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
@@ -2721,19 +2789,20 @@
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20" s="8"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="4"/>
-      <c r="G21" s="8"/>
+      <c r="F21" s="4"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="8"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="14"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
@@ -2744,19 +2813,20 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U21" s="8"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="4"/>
-      <c r="G22" s="8"/>
+      <c r="F22" s="4"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="8"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="14"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
@@ -2767,19 +2837,20 @@
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U22" s="8"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="4"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="4"/>
-      <c r="G23" s="8"/>
+      <c r="F23" s="4"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="8"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="14"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
@@ -2790,19 +2861,20 @@
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
       <c r="T23" s="8"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U23" s="8"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="4"/>
-      <c r="G24" s="8"/>
+      <c r="F24" s="4"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="8"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="14"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
@@ -2813,19 +2885,20 @@
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24" s="8"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="4"/>
-      <c r="G25" s="8"/>
+      <c r="F25" s="4"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="8"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="14"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
@@ -2836,19 +2909,20 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U25" s="8"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="4"/>
-      <c r="G26" s="8"/>
+      <c r="F26" s="4"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="8"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="14"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
@@ -2859,19 +2933,20 @@
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U26" s="8"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="4"/>
-      <c r="G27" s="8"/>
+      <c r="F27" s="4"/>
       <c r="H27" s="8"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="8"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="14"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
@@ -2882,19 +2957,20 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U27" s="8"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="4"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="4"/>
-      <c r="G28" s="8"/>
+      <c r="F28" s="4"/>
       <c r="H28" s="8"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="8"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="14"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
@@ -2905,19 +2981,20 @@
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U28" s="8"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="4"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="4"/>
-      <c r="G29" s="8"/>
+      <c r="F29" s="4"/>
       <c r="H29" s="8"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="8"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="14"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
@@ -2928,19 +3005,20 @@
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U29" s="8"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="4"/>
-      <c r="G30" s="8"/>
+      <c r="F30" s="4"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="8"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="14"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
@@ -2951,19 +3029,20 @@
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
       <c r="T30" s="8"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U30" s="8"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="9"/>
       <c r="E31" s="4"/>
-      <c r="G31" s="8"/>
+      <c r="F31" s="4"/>
       <c r="H31" s="8"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="8"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="14"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
@@ -2974,19 +3053,20 @@
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
       <c r="T31" s="8"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U31" s="8"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="4"/>
+      <c r="D32" s="9"/>
       <c r="E32" s="4"/>
-      <c r="G32" s="8"/>
+      <c r="F32" s="4"/>
       <c r="H32" s="8"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="8"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="14"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
@@ -2997,15 +3077,20 @@
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
-    </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U32" s="8"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>31</v>
+      </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="4"/>
+      <c r="D33" s="9"/>
       <c r="E33" s="4"/>
-      <c r="G33" s="8"/>
+      <c r="F33" s="4"/>
       <c r="H33" s="8"/>
-      <c r="J33" s="8"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="14"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
@@ -3016,15 +3101,16 @@
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
       <c r="T33" s="8"/>
-    </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U33" s="8"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="4"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="4"/>
-      <c r="G34" s="8"/>
+      <c r="F34" s="4"/>
       <c r="H34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="I34" s="9"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
@@ -3035,15 +3121,16 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
-    </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U34" s="8"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="9"/>
       <c r="E35" s="4"/>
-      <c r="G35" s="8"/>
+      <c r="F35" s="4"/>
       <c r="H35" s="8"/>
-      <c r="J35" s="8"/>
+      <c r="I35" s="9"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
@@ -3054,15 +3141,16 @@
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
       <c r="T35" s="8"/>
-    </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U35" s="8"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="4"/>
+      <c r="D36" s="9"/>
       <c r="E36" s="4"/>
-      <c r="G36" s="8"/>
+      <c r="F36" s="4"/>
       <c r="H36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="I36" s="9"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
@@ -3073,15 +3161,16 @@
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
-    </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U36" s="8"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="4"/>
+      <c r="D37" s="9"/>
       <c r="E37" s="4"/>
-      <c r="G37" s="8"/>
+      <c r="F37" s="4"/>
       <c r="H37" s="8"/>
-      <c r="J37" s="8"/>
+      <c r="I37" s="9"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
@@ -3092,15 +3181,16 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
       <c r="T37" s="8"/>
-    </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U37" s="8"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="4"/>
+      <c r="D38" s="9"/>
       <c r="E38" s="4"/>
-      <c r="G38" s="8"/>
+      <c r="F38" s="4"/>
       <c r="H38" s="8"/>
-      <c r="J38" s="8"/>
+      <c r="I38" s="9"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
@@ -3111,15 +3201,16 @@
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
       <c r="T38" s="8"/>
-    </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U38" s="8"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="4"/>
+      <c r="D39" s="9"/>
       <c r="E39" s="4"/>
-      <c r="G39" s="8"/>
+      <c r="F39" s="4"/>
       <c r="H39" s="8"/>
-      <c r="J39" s="8"/>
+      <c r="I39" s="9"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
@@ -3130,15 +3221,16 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
       <c r="T39" s="8"/>
-    </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U39" s="8"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="4"/>
+      <c r="D40" s="9"/>
       <c r="E40" s="4"/>
-      <c r="G40" s="8"/>
+      <c r="F40" s="4"/>
       <c r="H40" s="8"/>
-      <c r="J40" s="8"/>
+      <c r="I40" s="9"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
@@ -3149,15 +3241,16 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
       <c r="T40" s="8"/>
-    </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U40" s="8"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="4"/>
-      <c r="G41" s="8"/>
+      <c r="F41" s="4"/>
       <c r="H41" s="8"/>
-      <c r="J41" s="8"/>
+      <c r="I41" s="9"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
@@ -3168,15 +3261,16 @@
       <c r="R41" s="8"/>
       <c r="S41" s="8"/>
       <c r="T41" s="8"/>
-    </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U41" s="8"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="4"/>
+      <c r="D42" s="9"/>
       <c r="E42" s="4"/>
-      <c r="G42" s="8"/>
+      <c r="F42" s="4"/>
       <c r="H42" s="8"/>
-      <c r="J42" s="8"/>
+      <c r="I42" s="9"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
@@ -3187,15 +3281,16 @@
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
       <c r="T42" s="8"/>
-    </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U42" s="8"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="4"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="4"/>
-      <c r="G43" s="8"/>
+      <c r="F43" s="4"/>
       <c r="H43" s="8"/>
-      <c r="J43" s="8"/>
+      <c r="I43" s="9"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
@@ -3206,15 +3301,16 @@
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
       <c r="T43" s="8"/>
-    </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U43" s="8"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="4"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="4"/>
-      <c r="G44" s="8"/>
+      <c r="F44" s="4"/>
       <c r="H44" s="8"/>
-      <c r="J44" s="8"/>
+      <c r="I44" s="9"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
@@ -3225,15 +3321,16 @@
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
       <c r="T44" s="8"/>
-    </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U44" s="8"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="4"/>
+      <c r="D45" s="9"/>
       <c r="E45" s="4"/>
-      <c r="G45" s="8"/>
+      <c r="F45" s="4"/>
       <c r="H45" s="8"/>
-      <c r="J45" s="8"/>
+      <c r="I45" s="9"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
@@ -3244,15 +3341,16 @@
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
       <c r="T45" s="8"/>
-    </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U45" s="8"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="4"/>
+      <c r="D46" s="9"/>
       <c r="E46" s="4"/>
-      <c r="G46" s="8"/>
+      <c r="F46" s="4"/>
       <c r="H46" s="8"/>
-      <c r="J46" s="8"/>
+      <c r="I46" s="9"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
@@ -3263,15 +3361,16 @@
       <c r="R46" s="8"/>
       <c r="S46" s="8"/>
       <c r="T46" s="8"/>
-    </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U46" s="8"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="4"/>
+      <c r="D47" s="9"/>
       <c r="E47" s="4"/>
-      <c r="G47" s="8"/>
+      <c r="F47" s="4"/>
       <c r="H47" s="8"/>
-      <c r="J47" s="8"/>
+      <c r="I47" s="9"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
@@ -3282,15 +3381,16 @@
       <c r="R47" s="8"/>
       <c r="S47" s="8"/>
       <c r="T47" s="8"/>
-    </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U47" s="8"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="4"/>
+      <c r="D48" s="9"/>
       <c r="E48" s="4"/>
-      <c r="G48" s="8"/>
+      <c r="F48" s="4"/>
       <c r="H48" s="8"/>
-      <c r="J48" s="8"/>
+      <c r="I48" s="9"/>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
@@ -3301,15 +3401,16 @@
       <c r="R48" s="8"/>
       <c r="S48" s="8"/>
       <c r="T48" s="8"/>
-    </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U48" s="8"/>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="4"/>
+      <c r="D49" s="9"/>
       <c r="E49" s="4"/>
-      <c r="G49" s="8"/>
+      <c r="F49" s="4"/>
       <c r="H49" s="8"/>
-      <c r="J49" s="8"/>
+      <c r="I49" s="9"/>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
@@ -3320,15 +3421,16 @@
       <c r="R49" s="8"/>
       <c r="S49" s="8"/>
       <c r="T49" s="8"/>
-    </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U49" s="8"/>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="4"/>
+      <c r="D50" s="9"/>
       <c r="E50" s="4"/>
-      <c r="G50" s="8"/>
+      <c r="F50" s="4"/>
       <c r="H50" s="8"/>
-      <c r="J50" s="8"/>
+      <c r="I50" s="9"/>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
@@ -3339,15 +3441,16 @@
       <c r="R50" s="8"/>
       <c r="S50" s="8"/>
       <c r="T50" s="8"/>
-    </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U50" s="8"/>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="4"/>
+      <c r="D51" s="9"/>
       <c r="E51" s="4"/>
-      <c r="G51" s="8"/>
+      <c r="F51" s="4"/>
       <c r="H51" s="8"/>
-      <c r="J51" s="8"/>
+      <c r="I51" s="9"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
@@ -3358,15 +3461,16 @@
       <c r="R51" s="8"/>
       <c r="S51" s="8"/>
       <c r="T51" s="8"/>
-    </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U51" s="8"/>
+    </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="4"/>
+      <c r="D52" s="9"/>
       <c r="E52" s="4"/>
-      <c r="G52" s="8"/>
+      <c r="F52" s="4"/>
       <c r="H52" s="8"/>
-      <c r="J52" s="8"/>
+      <c r="I52" s="9"/>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
@@ -3377,15 +3481,16 @@
       <c r="R52" s="8"/>
       <c r="S52" s="8"/>
       <c r="T52" s="8"/>
-    </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U52" s="8"/>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="4"/>
+      <c r="D53" s="9"/>
       <c r="E53" s="4"/>
-      <c r="G53" s="8"/>
+      <c r="F53" s="4"/>
       <c r="H53" s="8"/>
-      <c r="J53" s="8"/>
+      <c r="I53" s="9"/>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
@@ -3396,15 +3501,16 @@
       <c r="R53" s="8"/>
       <c r="S53" s="8"/>
       <c r="T53" s="8"/>
-    </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U53" s="8"/>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="4"/>
+      <c r="D54" s="9"/>
       <c r="E54" s="4"/>
-      <c r="G54" s="8"/>
+      <c r="F54" s="4"/>
       <c r="H54" s="8"/>
-      <c r="J54" s="8"/>
+      <c r="I54" s="9"/>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
@@ -3415,15 +3521,16 @@
       <c r="R54" s="8"/>
       <c r="S54" s="8"/>
       <c r="T54" s="8"/>
-    </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U54" s="8"/>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="4"/>
+      <c r="D55" s="9"/>
       <c r="E55" s="4"/>
-      <c r="G55" s="8"/>
+      <c r="F55" s="4"/>
       <c r="H55" s="8"/>
-      <c r="J55" s="8"/>
+      <c r="I55" s="9"/>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
@@ -3434,15 +3541,16 @@
       <c r="R55" s="8"/>
       <c r="S55" s="8"/>
       <c r="T55" s="8"/>
-    </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U55" s="8"/>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="4"/>
+      <c r="D56" s="9"/>
       <c r="E56" s="4"/>
-      <c r="G56" s="8"/>
+      <c r="F56" s="4"/>
       <c r="H56" s="8"/>
-      <c r="J56" s="8"/>
+      <c r="I56" s="9"/>
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
@@ -3453,15 +3561,16 @@
       <c r="R56" s="8"/>
       <c r="S56" s="8"/>
       <c r="T56" s="8"/>
-    </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U56" s="8"/>
+    </row>
+    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
-      <c r="D57" s="4"/>
+      <c r="D57" s="9"/>
       <c r="E57" s="4"/>
-      <c r="G57" s="8"/>
+      <c r="F57" s="4"/>
       <c r="H57" s="8"/>
-      <c r="J57" s="8"/>
+      <c r="I57" s="9"/>
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
@@ -3472,15 +3581,16 @@
       <c r="R57" s="8"/>
       <c r="S57" s="8"/>
       <c r="T57" s="8"/>
-    </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U57" s="8"/>
+    </row>
+    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="4"/>
+      <c r="D58" s="9"/>
       <c r="E58" s="4"/>
-      <c r="G58" s="8"/>
+      <c r="F58" s="4"/>
       <c r="H58" s="8"/>
-      <c r="J58" s="8"/>
+      <c r="I58" s="9"/>
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
@@ -3491,15 +3601,16 @@
       <c r="R58" s="8"/>
       <c r="S58" s="8"/>
       <c r="T58" s="8"/>
-    </row>
-    <row r="59" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U58" s="8"/>
+    </row>
+    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="4"/>
+      <c r="D59" s="9"/>
       <c r="E59" s="4"/>
-      <c r="G59" s="8"/>
+      <c r="F59" s="4"/>
       <c r="H59" s="8"/>
-      <c r="J59" s="8"/>
+      <c r="I59" s="9"/>
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
       <c r="M59" s="8"/>
@@ -3510,15 +3621,16 @@
       <c r="R59" s="8"/>
       <c r="S59" s="8"/>
       <c r="T59" s="8"/>
-    </row>
-    <row r="60" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U59" s="8"/>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="4"/>
+      <c r="D60" s="9"/>
       <c r="E60" s="4"/>
-      <c r="G60" s="8"/>
+      <c r="F60" s="4"/>
       <c r="H60" s="8"/>
-      <c r="J60" s="8"/>
+      <c r="I60" s="9"/>
       <c r="K60" s="8"/>
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
@@ -3529,15 +3641,16 @@
       <c r="R60" s="8"/>
       <c r="S60" s="8"/>
       <c r="T60" s="8"/>
-    </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U60" s="8"/>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="4"/>
+      <c r="D61" s="9"/>
       <c r="E61" s="4"/>
-      <c r="G61" s="8"/>
+      <c r="F61" s="4"/>
       <c r="H61" s="8"/>
-      <c r="J61" s="8"/>
+      <c r="I61" s="9"/>
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
@@ -3548,15 +3661,16 @@
       <c r="R61" s="8"/>
       <c r="S61" s="8"/>
       <c r="T61" s="8"/>
-    </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U61" s="8"/>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="4"/>
+      <c r="D62" s="9"/>
       <c r="E62" s="4"/>
-      <c r="G62" s="8"/>
+      <c r="F62" s="4"/>
       <c r="H62" s="8"/>
-      <c r="J62" s="8"/>
+      <c r="I62" s="9"/>
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
       <c r="M62" s="8"/>
@@ -3567,15 +3681,16 @@
       <c r="R62" s="8"/>
       <c r="S62" s="8"/>
       <c r="T62" s="8"/>
-    </row>
-    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U62" s="8"/>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="4"/>
+      <c r="D63" s="9"/>
       <c r="E63" s="4"/>
-      <c r="G63" s="8"/>
+      <c r="F63" s="4"/>
       <c r="H63" s="8"/>
-      <c r="J63" s="8"/>
+      <c r="I63" s="9"/>
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
@@ -3586,15 +3701,16 @@
       <c r="R63" s="8"/>
       <c r="S63" s="8"/>
       <c r="T63" s="8"/>
-    </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U63" s="8"/>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="4"/>
+      <c r="D64" s="9"/>
       <c r="E64" s="4"/>
-      <c r="G64" s="8"/>
+      <c r="F64" s="4"/>
       <c r="H64" s="8"/>
-      <c r="J64" s="8"/>
+      <c r="I64" s="9"/>
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
       <c r="M64" s="8"/>
@@ -3605,15 +3721,16 @@
       <c r="R64" s="8"/>
       <c r="S64" s="8"/>
       <c r="T64" s="8"/>
-    </row>
-    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U64" s="8"/>
+    </row>
+    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="4"/>
+      <c r="D65" s="9"/>
       <c r="E65" s="4"/>
-      <c r="G65" s="8"/>
+      <c r="F65" s="4"/>
       <c r="H65" s="8"/>
-      <c r="J65" s="8"/>
+      <c r="I65" s="9"/>
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
       <c r="M65" s="8"/>
@@ -3624,15 +3741,16 @@
       <c r="R65" s="8"/>
       <c r="S65" s="8"/>
       <c r="T65" s="8"/>
-    </row>
-    <row r="66" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U65" s="8"/>
+    </row>
+    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="4"/>
+      <c r="D66" s="9"/>
       <c r="E66" s="4"/>
-      <c r="G66" s="8"/>
+      <c r="F66" s="4"/>
       <c r="H66" s="8"/>
-      <c r="J66" s="8"/>
+      <c r="I66" s="9"/>
       <c r="K66" s="8"/>
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
@@ -3643,15 +3761,16 @@
       <c r="R66" s="8"/>
       <c r="S66" s="8"/>
       <c r="T66" s="8"/>
-    </row>
-    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U66" s="8"/>
+    </row>
+    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="4"/>
+      <c r="D67" s="9"/>
       <c r="E67" s="4"/>
-      <c r="G67" s="8"/>
+      <c r="F67" s="4"/>
       <c r="H67" s="8"/>
-      <c r="J67" s="8"/>
+      <c r="I67" s="9"/>
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
       <c r="M67" s="8"/>
@@ -3662,15 +3781,16 @@
       <c r="R67" s="8"/>
       <c r="S67" s="8"/>
       <c r="T67" s="8"/>
-    </row>
-    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U67" s="8"/>
+    </row>
+    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="4"/>
+      <c r="D68" s="9"/>
       <c r="E68" s="4"/>
-      <c r="G68" s="8"/>
+      <c r="F68" s="4"/>
       <c r="H68" s="8"/>
-      <c r="J68" s="8"/>
+      <c r="I68" s="9"/>
       <c r="K68" s="8"/>
       <c r="L68" s="8"/>
       <c r="M68" s="8"/>
@@ -3681,15 +3801,16 @@
       <c r="R68" s="8"/>
       <c r="S68" s="8"/>
       <c r="T68" s="8"/>
-    </row>
-    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U68" s="8"/>
+    </row>
+    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="4"/>
+      <c r="D69" s="9"/>
       <c r="E69" s="4"/>
-      <c r="G69" s="8"/>
+      <c r="F69" s="4"/>
       <c r="H69" s="8"/>
-      <c r="J69" s="8"/>
+      <c r="I69" s="9"/>
       <c r="K69" s="8"/>
       <c r="L69" s="8"/>
       <c r="M69" s="8"/>
@@ -3700,15 +3821,16 @@
       <c r="R69" s="8"/>
       <c r="S69" s="8"/>
       <c r="T69" s="8"/>
-    </row>
-    <row r="70" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U69" s="8"/>
+    </row>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="4"/>
+      <c r="D70" s="9"/>
       <c r="E70" s="4"/>
-      <c r="G70" s="8"/>
+      <c r="F70" s="4"/>
       <c r="H70" s="8"/>
-      <c r="J70" s="8"/>
+      <c r="I70" s="9"/>
       <c r="K70" s="8"/>
       <c r="L70" s="8"/>
       <c r="M70" s="8"/>
@@ -3719,15 +3841,16 @@
       <c r="R70" s="8"/>
       <c r="S70" s="8"/>
       <c r="T70" s="8"/>
-    </row>
-    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U70" s="8"/>
+    </row>
+    <row r="71" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="4"/>
+      <c r="D71" s="9"/>
       <c r="E71" s="4"/>
-      <c r="G71" s="8"/>
+      <c r="F71" s="4"/>
       <c r="H71" s="8"/>
-      <c r="J71" s="8"/>
+      <c r="I71" s="9"/>
       <c r="K71" s="8"/>
       <c r="L71" s="8"/>
       <c r="M71" s="8"/>
@@ -3738,15 +3861,16 @@
       <c r="R71" s="8"/>
       <c r="S71" s="8"/>
       <c r="T71" s="8"/>
-    </row>
-    <row r="72" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U71" s="8"/>
+    </row>
+    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="4"/>
+      <c r="D72" s="9"/>
       <c r="E72" s="4"/>
-      <c r="G72" s="8"/>
+      <c r="F72" s="4"/>
       <c r="H72" s="8"/>
-      <c r="J72" s="8"/>
+      <c r="I72" s="9"/>
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="M72" s="8"/>
@@ -3757,15 +3881,16 @@
       <c r="R72" s="8"/>
       <c r="S72" s="8"/>
       <c r="T72" s="8"/>
-    </row>
-    <row r="73" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U72" s="8"/>
+    </row>
+    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="4"/>
+      <c r="D73" s="9"/>
       <c r="E73" s="4"/>
-      <c r="G73" s="8"/>
+      <c r="F73" s="4"/>
       <c r="H73" s="8"/>
-      <c r="J73" s="8"/>
+      <c r="I73" s="9"/>
       <c r="K73" s="8"/>
       <c r="L73" s="8"/>
       <c r="M73" s="8"/>
@@ -3776,15 +3901,16 @@
       <c r="R73" s="8"/>
       <c r="S73" s="8"/>
       <c r="T73" s="8"/>
-    </row>
-    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U73" s="8"/>
+    </row>
+    <row r="74" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="4"/>
+      <c r="D74" s="9"/>
       <c r="E74" s="4"/>
-      <c r="G74" s="8"/>
+      <c r="F74" s="4"/>
       <c r="H74" s="8"/>
-      <c r="J74" s="8"/>
+      <c r="I74" s="9"/>
       <c r="K74" s="8"/>
       <c r="L74" s="8"/>
       <c r="M74" s="8"/>
@@ -3795,15 +3921,16 @@
       <c r="R74" s="8"/>
       <c r="S74" s="8"/>
       <c r="T74" s="8"/>
-    </row>
-    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U74" s="8"/>
+    </row>
+    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="4"/>
+      <c r="D75" s="9"/>
       <c r="E75" s="4"/>
-      <c r="G75" s="8"/>
+      <c r="F75" s="4"/>
       <c r="H75" s="8"/>
-      <c r="J75" s="8"/>
+      <c r="I75" s="9"/>
       <c r="K75" s="8"/>
       <c r="L75" s="8"/>
       <c r="M75" s="8"/>
@@ -3814,15 +3941,16 @@
       <c r="R75" s="8"/>
       <c r="S75" s="8"/>
       <c r="T75" s="8"/>
-    </row>
-    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U75" s="8"/>
+    </row>
+    <row r="76" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="4"/>
+      <c r="D76" s="9"/>
       <c r="E76" s="4"/>
-      <c r="G76" s="8"/>
+      <c r="F76" s="4"/>
       <c r="H76" s="8"/>
-      <c r="J76" s="8"/>
+      <c r="I76" s="9"/>
       <c r="K76" s="8"/>
       <c r="L76" s="8"/>
       <c r="M76" s="8"/>
@@ -3833,15 +3961,16 @@
       <c r="R76" s="8"/>
       <c r="S76" s="8"/>
       <c r="T76" s="8"/>
-    </row>
-    <row r="77" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U76" s="8"/>
+    </row>
+    <row r="77" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="4"/>
+      <c r="D77" s="9"/>
       <c r="E77" s="4"/>
-      <c r="G77" s="8"/>
+      <c r="F77" s="4"/>
       <c r="H77" s="8"/>
-      <c r="J77" s="8"/>
+      <c r="I77" s="9"/>
       <c r="K77" s="8"/>
       <c r="L77" s="8"/>
       <c r="M77" s="8"/>
@@ -3852,15 +3981,16 @@
       <c r="R77" s="8"/>
       <c r="S77" s="8"/>
       <c r="T77" s="8"/>
-    </row>
-    <row r="78" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U77" s="8"/>
+    </row>
+    <row r="78" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="4"/>
+      <c r="D78" s="9"/>
       <c r="E78" s="4"/>
-      <c r="G78" s="8"/>
+      <c r="F78" s="4"/>
       <c r="H78" s="8"/>
-      <c r="J78" s="8"/>
+      <c r="I78" s="9"/>
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
@@ -3871,15 +4001,16 @@
       <c r="R78" s="8"/>
       <c r="S78" s="8"/>
       <c r="T78" s="8"/>
-    </row>
-    <row r="79" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U78" s="8"/>
+    </row>
+    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="4"/>
+      <c r="D79" s="9"/>
       <c r="E79" s="4"/>
-      <c r="G79" s="8"/>
+      <c r="F79" s="4"/>
       <c r="H79" s="8"/>
-      <c r="J79" s="8"/>
+      <c r="I79" s="9"/>
       <c r="K79" s="8"/>
       <c r="L79" s="8"/>
       <c r="M79" s="8"/>
@@ -3890,15 +4021,16 @@
       <c r="R79" s="8"/>
       <c r="S79" s="8"/>
       <c r="T79" s="8"/>
-    </row>
-    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U79" s="8"/>
+    </row>
+    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="4"/>
+      <c r="D80" s="9"/>
       <c r="E80" s="4"/>
-      <c r="G80" s="8"/>
+      <c r="F80" s="4"/>
       <c r="H80" s="8"/>
-      <c r="J80" s="8"/>
+      <c r="I80" s="9"/>
       <c r="K80" s="8"/>
       <c r="L80" s="8"/>
       <c r="M80" s="8"/>
@@ -3909,15 +4041,16 @@
       <c r="R80" s="8"/>
       <c r="S80" s="8"/>
       <c r="T80" s="8"/>
-    </row>
-    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U80" s="8"/>
+    </row>
+    <row r="81" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
-      <c r="D81" s="4"/>
+      <c r="D81" s="9"/>
       <c r="E81" s="4"/>
-      <c r="G81" s="8"/>
+      <c r="F81" s="4"/>
       <c r="H81" s="8"/>
-      <c r="J81" s="8"/>
+      <c r="I81" s="9"/>
       <c r="K81" s="8"/>
       <c r="L81" s="8"/>
       <c r="M81" s="8"/>
@@ -3928,15 +4061,16 @@
       <c r="R81" s="8"/>
       <c r="S81" s="8"/>
       <c r="T81" s="8"/>
-    </row>
-    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U81" s="8"/>
+    </row>
+    <row r="82" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
-      <c r="D82" s="4"/>
+      <c r="D82" s="9"/>
       <c r="E82" s="4"/>
-      <c r="G82" s="8"/>
+      <c r="F82" s="4"/>
       <c r="H82" s="8"/>
-      <c r="J82" s="8"/>
+      <c r="I82" s="9"/>
       <c r="K82" s="8"/>
       <c r="L82" s="8"/>
       <c r="M82" s="8"/>
@@ -3947,15 +4081,16 @@
       <c r="R82" s="8"/>
       <c r="S82" s="8"/>
       <c r="T82" s="8"/>
-    </row>
-    <row r="83" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U82" s="8"/>
+    </row>
+    <row r="83" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="4"/>
+      <c r="D83" s="9"/>
       <c r="E83" s="4"/>
-      <c r="G83" s="8"/>
+      <c r="F83" s="4"/>
       <c r="H83" s="8"/>
-      <c r="J83" s="8"/>
+      <c r="I83" s="9"/>
       <c r="K83" s="8"/>
       <c r="L83" s="8"/>
       <c r="M83" s="8"/>
@@ -3966,15 +4101,16 @@
       <c r="R83" s="8"/>
       <c r="S83" s="8"/>
       <c r="T83" s="8"/>
-    </row>
-    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U83" s="8"/>
+    </row>
+    <row r="84" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
-      <c r="D84" s="4"/>
+      <c r="D84" s="9"/>
       <c r="E84" s="4"/>
-      <c r="G84" s="8"/>
+      <c r="F84" s="4"/>
       <c r="H84" s="8"/>
-      <c r="J84" s="8"/>
+      <c r="I84" s="9"/>
       <c r="K84" s="8"/>
       <c r="L84" s="8"/>
       <c r="M84" s="8"/>
@@ -3985,15 +4121,16 @@
       <c r="R84" s="8"/>
       <c r="S84" s="8"/>
       <c r="T84" s="8"/>
-    </row>
-    <row r="85" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U84" s="8"/>
+    </row>
+    <row r="85" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
-      <c r="D85" s="4"/>
+      <c r="D85" s="9"/>
       <c r="E85" s="4"/>
-      <c r="G85" s="8"/>
+      <c r="F85" s="4"/>
       <c r="H85" s="8"/>
-      <c r="J85" s="8"/>
+      <c r="I85" s="9"/>
       <c r="K85" s="8"/>
       <c r="L85" s="8"/>
       <c r="M85" s="8"/>
@@ -4004,15 +4141,16 @@
       <c r="R85" s="8"/>
       <c r="S85" s="8"/>
       <c r="T85" s="8"/>
-    </row>
-    <row r="86" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U85" s="8"/>
+    </row>
+    <row r="86" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
-      <c r="D86" s="4"/>
+      <c r="D86" s="9"/>
       <c r="E86" s="4"/>
-      <c r="G86" s="8"/>
+      <c r="F86" s="4"/>
       <c r="H86" s="8"/>
-      <c r="J86" s="8"/>
+      <c r="I86" s="9"/>
       <c r="K86" s="8"/>
       <c r="L86" s="8"/>
       <c r="M86" s="8"/>
@@ -4023,15 +4161,16 @@
       <c r="R86" s="8"/>
       <c r="S86" s="8"/>
       <c r="T86" s="8"/>
-    </row>
-    <row r="87" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U86" s="8"/>
+    </row>
+    <row r="87" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
-      <c r="D87" s="4"/>
+      <c r="D87" s="9"/>
       <c r="E87" s="4"/>
-      <c r="G87" s="8"/>
+      <c r="F87" s="4"/>
       <c r="H87" s="8"/>
-      <c r="J87" s="8"/>
+      <c r="I87" s="9"/>
       <c r="K87" s="8"/>
       <c r="L87" s="8"/>
       <c r="M87" s="8"/>
@@ -4042,15 +4181,16 @@
       <c r="R87" s="8"/>
       <c r="S87" s="8"/>
       <c r="T87" s="8"/>
-    </row>
-    <row r="88" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U87" s="8"/>
+    </row>
+    <row r="88" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="4"/>
+      <c r="D88" s="9"/>
       <c r="E88" s="4"/>
-      <c r="G88" s="8"/>
+      <c r="F88" s="4"/>
       <c r="H88" s="8"/>
-      <c r="J88" s="8"/>
+      <c r="I88" s="9"/>
       <c r="K88" s="8"/>
       <c r="L88" s="8"/>
       <c r="M88" s="8"/>
@@ -4061,15 +4201,16 @@
       <c r="R88" s="8"/>
       <c r="S88" s="8"/>
       <c r="T88" s="8"/>
-    </row>
-    <row r="89" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U88" s="8"/>
+    </row>
+    <row r="89" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
-      <c r="D89" s="4"/>
+      <c r="D89" s="9"/>
       <c r="E89" s="4"/>
-      <c r="G89" s="8"/>
+      <c r="F89" s="4"/>
       <c r="H89" s="8"/>
-      <c r="J89" s="8"/>
+      <c r="I89" s="9"/>
       <c r="K89" s="8"/>
       <c r="L89" s="8"/>
       <c r="M89" s="8"/>
@@ -4080,15 +4221,16 @@
       <c r="R89" s="8"/>
       <c r="S89" s="8"/>
       <c r="T89" s="8"/>
-    </row>
-    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U89" s="8"/>
+    </row>
+    <row r="90" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
-      <c r="D90" s="4"/>
+      <c r="D90" s="9"/>
       <c r="E90" s="4"/>
-      <c r="G90" s="8"/>
+      <c r="F90" s="4"/>
       <c r="H90" s="8"/>
-      <c r="J90" s="8"/>
+      <c r="I90" s="9"/>
       <c r="K90" s="8"/>
       <c r="L90" s="8"/>
       <c r="M90" s="8"/>
@@ -4099,15 +4241,16 @@
       <c r="R90" s="8"/>
       <c r="S90" s="8"/>
       <c r="T90" s="8"/>
-    </row>
-    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U90" s="8"/>
+    </row>
+    <row r="91" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
-      <c r="D91" s="4"/>
+      <c r="D91" s="9"/>
       <c r="E91" s="4"/>
-      <c r="G91" s="8"/>
+      <c r="F91" s="4"/>
       <c r="H91" s="8"/>
-      <c r="J91" s="8"/>
+      <c r="I91" s="9"/>
       <c r="K91" s="8"/>
       <c r="L91" s="8"/>
       <c r="M91" s="8"/>
@@ -4118,15 +4261,16 @@
       <c r="R91" s="8"/>
       <c r="S91" s="8"/>
       <c r="T91" s="8"/>
-    </row>
-    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U91" s="8"/>
+    </row>
+    <row r="92" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
-      <c r="D92" s="4"/>
+      <c r="D92" s="9"/>
       <c r="E92" s="4"/>
-      <c r="G92" s="8"/>
+      <c r="F92" s="4"/>
       <c r="H92" s="8"/>
-      <c r="J92" s="8"/>
+      <c r="I92" s="9"/>
       <c r="K92" s="8"/>
       <c r="L92" s="8"/>
       <c r="M92" s="8"/>
@@ -4137,15 +4281,16 @@
       <c r="R92" s="8"/>
       <c r="S92" s="8"/>
       <c r="T92" s="8"/>
-    </row>
-    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U92" s="8"/>
+    </row>
+    <row r="93" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
-      <c r="D93" s="4"/>
+      <c r="D93" s="9"/>
       <c r="E93" s="4"/>
-      <c r="G93" s="8"/>
+      <c r="F93" s="4"/>
       <c r="H93" s="8"/>
-      <c r="J93" s="8"/>
+      <c r="I93" s="9"/>
       <c r="K93" s="8"/>
       <c r="L93" s="8"/>
       <c r="M93" s="8"/>
@@ -4156,15 +4301,16 @@
       <c r="R93" s="8"/>
       <c r="S93" s="8"/>
       <c r="T93" s="8"/>
-    </row>
-    <row r="94" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U93" s="8"/>
+    </row>
+    <row r="94" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
-      <c r="D94" s="4"/>
+      <c r="D94" s="9"/>
       <c r="E94" s="4"/>
-      <c r="G94" s="8"/>
+      <c r="F94" s="4"/>
       <c r="H94" s="8"/>
-      <c r="J94" s="8"/>
+      <c r="I94" s="9"/>
       <c r="K94" s="8"/>
       <c r="L94" s="8"/>
       <c r="M94" s="8"/>
@@ -4175,15 +4321,16 @@
       <c r="R94" s="8"/>
       <c r="S94" s="8"/>
       <c r="T94" s="8"/>
-    </row>
-    <row r="95" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U94" s="8"/>
+    </row>
+    <row r="95" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
-      <c r="D95" s="4"/>
+      <c r="D95" s="9"/>
       <c r="E95" s="4"/>
-      <c r="G95" s="8"/>
+      <c r="F95" s="4"/>
       <c r="H95" s="8"/>
-      <c r="J95" s="8"/>
+      <c r="I95" s="9"/>
       <c r="K95" s="8"/>
       <c r="L95" s="8"/>
       <c r="M95" s="8"/>
@@ -4194,15 +4341,16 @@
       <c r="R95" s="8"/>
       <c r="S95" s="8"/>
       <c r="T95" s="8"/>
-    </row>
-    <row r="96" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U95" s="8"/>
+    </row>
+    <row r="96" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="4"/>
+      <c r="D96" s="9"/>
       <c r="E96" s="4"/>
-      <c r="G96" s="8"/>
+      <c r="F96" s="4"/>
       <c r="H96" s="8"/>
-      <c r="J96" s="8"/>
+      <c r="I96" s="9"/>
       <c r="K96" s="8"/>
       <c r="L96" s="8"/>
       <c r="M96" s="8"/>
@@ -4213,15 +4361,16 @@
       <c r="R96" s="8"/>
       <c r="S96" s="8"/>
       <c r="T96" s="8"/>
-    </row>
-    <row r="97" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U96" s="8"/>
+    </row>
+    <row r="97" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="4"/>
+      <c r="D97" s="9"/>
       <c r="E97" s="4"/>
-      <c r="G97" s="8"/>
+      <c r="F97" s="4"/>
       <c r="H97" s="8"/>
-      <c r="J97" s="8"/>
+      <c r="I97" s="9"/>
       <c r="K97" s="8"/>
       <c r="L97" s="8"/>
       <c r="M97" s="8"/>
@@ -4232,15 +4381,16 @@
       <c r="R97" s="8"/>
       <c r="S97" s="8"/>
       <c r="T97" s="8"/>
-    </row>
-    <row r="98" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U97" s="8"/>
+    </row>
+    <row r="98" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="4"/>
+      <c r="D98" s="9"/>
       <c r="E98" s="4"/>
-      <c r="G98" s="8"/>
+      <c r="F98" s="4"/>
       <c r="H98" s="8"/>
-      <c r="J98" s="8"/>
+      <c r="I98" s="9"/>
       <c r="K98" s="8"/>
       <c r="L98" s="8"/>
       <c r="M98" s="8"/>
@@ -4251,15 +4401,16 @@
       <c r="R98" s="8"/>
       <c r="S98" s="8"/>
       <c r="T98" s="8"/>
-    </row>
-    <row r="99" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U98" s="8"/>
+    </row>
+    <row r="99" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
-      <c r="D99" s="4"/>
+      <c r="D99" s="9"/>
       <c r="E99" s="4"/>
-      <c r="G99" s="8"/>
+      <c r="F99" s="4"/>
       <c r="H99" s="8"/>
-      <c r="J99" s="8"/>
+      <c r="I99" s="9"/>
       <c r="K99" s="8"/>
       <c r="L99" s="8"/>
       <c r="M99" s="8"/>
@@ -4270,15 +4421,16 @@
       <c r="R99" s="8"/>
       <c r="S99" s="8"/>
       <c r="T99" s="8"/>
-    </row>
-    <row r="100" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U99" s="8"/>
+    </row>
+    <row r="100" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
-      <c r="D100" s="4"/>
+      <c r="D100" s="9"/>
       <c r="E100" s="4"/>
-      <c r="G100" s="8"/>
+      <c r="F100" s="4"/>
       <c r="H100" s="8"/>
-      <c r="J100" s="8"/>
+      <c r="I100" s="9"/>
       <c r="K100" s="8"/>
       <c r="L100" s="8"/>
       <c r="M100" s="8"/>
@@ -4289,15 +4441,16 @@
       <c r="R100" s="8"/>
       <c r="S100" s="8"/>
       <c r="T100" s="8"/>
-    </row>
-    <row r="101" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U100" s="8"/>
+    </row>
+    <row r="101" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
-      <c r="D101" s="4"/>
+      <c r="D101" s="9"/>
       <c r="E101" s="4"/>
-      <c r="G101" s="8"/>
+      <c r="F101" s="4"/>
       <c r="H101" s="8"/>
-      <c r="J101" s="8"/>
+      <c r="I101" s="9"/>
       <c r="K101" s="8"/>
       <c r="L101" s="8"/>
       <c r="M101" s="8"/>
@@ -4308,15 +4461,16 @@
       <c r="R101" s="8"/>
       <c r="S101" s="8"/>
       <c r="T101" s="8"/>
-    </row>
-    <row r="102" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U101" s="8"/>
+    </row>
+    <row r="102" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
-      <c r="D102" s="4"/>
+      <c r="D102" s="9"/>
       <c r="E102" s="4"/>
-      <c r="G102" s="8"/>
+      <c r="F102" s="4"/>
       <c r="H102" s="8"/>
-      <c r="J102" s="8"/>
+      <c r="I102" s="9"/>
       <c r="K102" s="8"/>
       <c r="L102" s="8"/>
       <c r="M102" s="8"/>
@@ -4327,15 +4481,16 @@
       <c r="R102" s="8"/>
       <c r="S102" s="8"/>
       <c r="T102" s="8"/>
-    </row>
-    <row r="103" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U102" s="8"/>
+    </row>
+    <row r="103" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
-      <c r="D103" s="4"/>
+      <c r="D103" s="9"/>
       <c r="E103" s="4"/>
-      <c r="G103" s="8"/>
+      <c r="F103" s="4"/>
       <c r="H103" s="8"/>
-      <c r="J103" s="8"/>
+      <c r="I103" s="9"/>
       <c r="K103" s="8"/>
       <c r="L103" s="8"/>
       <c r="M103" s="8"/>
@@ -4346,15 +4501,16 @@
       <c r="R103" s="8"/>
       <c r="S103" s="8"/>
       <c r="T103" s="8"/>
-    </row>
-    <row r="104" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U103" s="8"/>
+    </row>
+    <row r="104" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
-      <c r="D104" s="4"/>
+      <c r="D104" s="9"/>
       <c r="E104" s="4"/>
-      <c r="G104" s="8"/>
+      <c r="F104" s="4"/>
       <c r="H104" s="8"/>
-      <c r="J104" s="8"/>
+      <c r="I104" s="9"/>
       <c r="K104" s="8"/>
       <c r="L104" s="8"/>
       <c r="M104" s="8"/>
@@ -4365,15 +4521,16 @@
       <c r="R104" s="8"/>
       <c r="S104" s="8"/>
       <c r="T104" s="8"/>
-    </row>
-    <row r="105" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U104" s="8"/>
+    </row>
+    <row r="105" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
-      <c r="D105" s="4"/>
+      <c r="D105" s="9"/>
       <c r="E105" s="4"/>
-      <c r="G105" s="8"/>
+      <c r="F105" s="4"/>
       <c r="H105" s="8"/>
-      <c r="J105" s="8"/>
+      <c r="I105" s="9"/>
       <c r="K105" s="8"/>
       <c r="L105" s="8"/>
       <c r="M105" s="8"/>
@@ -4384,15 +4541,16 @@
       <c r="R105" s="8"/>
       <c r="S105" s="8"/>
       <c r="T105" s="8"/>
-    </row>
-    <row r="106" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U105" s="8"/>
+    </row>
+    <row r="106" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
-      <c r="D106" s="4"/>
+      <c r="D106" s="9"/>
       <c r="E106" s="4"/>
-      <c r="G106" s="8"/>
+      <c r="F106" s="4"/>
       <c r="H106" s="8"/>
-      <c r="J106" s="8"/>
+      <c r="I106" s="9"/>
       <c r="K106" s="8"/>
       <c r="L106" s="8"/>
       <c r="M106" s="8"/>
@@ -4403,15 +4561,16 @@
       <c r="R106" s="8"/>
       <c r="S106" s="8"/>
       <c r="T106" s="8"/>
-    </row>
-    <row r="107" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U106" s="8"/>
+    </row>
+    <row r="107" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
-      <c r="D107" s="4"/>
+      <c r="D107" s="9"/>
       <c r="E107" s="4"/>
-      <c r="G107" s="8"/>
+      <c r="F107" s="4"/>
       <c r="H107" s="8"/>
-      <c r="J107" s="8"/>
+      <c r="I107" s="9"/>
       <c r="K107" s="8"/>
       <c r="L107" s="8"/>
       <c r="M107" s="8"/>
@@ -4422,15 +4581,16 @@
       <c r="R107" s="8"/>
       <c r="S107" s="8"/>
       <c r="T107" s="8"/>
-    </row>
-    <row r="108" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U107" s="8"/>
+    </row>
+    <row r="108" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
-      <c r="D108" s="4"/>
+      <c r="D108" s="9"/>
       <c r="E108" s="4"/>
-      <c r="G108" s="8"/>
+      <c r="F108" s="4"/>
       <c r="H108" s="8"/>
-      <c r="J108" s="8"/>
+      <c r="I108" s="9"/>
       <c r="K108" s="8"/>
       <c r="L108" s="8"/>
       <c r="M108" s="8"/>
@@ -4441,15 +4601,16 @@
       <c r="R108" s="8"/>
       <c r="S108" s="8"/>
       <c r="T108" s="8"/>
-    </row>
-    <row r="109" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U108" s="8"/>
+    </row>
+    <row r="109" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
-      <c r="D109" s="4"/>
+      <c r="D109" s="9"/>
       <c r="E109" s="4"/>
-      <c r="G109" s="8"/>
+      <c r="F109" s="4"/>
       <c r="H109" s="8"/>
-      <c r="J109" s="8"/>
+      <c r="I109" s="9"/>
       <c r="K109" s="8"/>
       <c r="L109" s="8"/>
       <c r="M109" s="8"/>
@@ -4460,15 +4621,16 @@
       <c r="R109" s="8"/>
       <c r="S109" s="8"/>
       <c r="T109" s="8"/>
-    </row>
-    <row r="110" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U109" s="8"/>
+    </row>
+    <row r="110" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
-      <c r="D110" s="4"/>
+      <c r="D110" s="9"/>
       <c r="E110" s="4"/>
-      <c r="G110" s="8"/>
+      <c r="F110" s="4"/>
       <c r="H110" s="8"/>
-      <c r="J110" s="8"/>
+      <c r="I110" s="9"/>
       <c r="K110" s="8"/>
       <c r="L110" s="8"/>
       <c r="M110" s="8"/>
@@ -4479,15 +4641,16 @@
       <c r="R110" s="8"/>
       <c r="S110" s="8"/>
       <c r="T110" s="8"/>
-    </row>
-    <row r="111" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U110" s="8"/>
+    </row>
+    <row r="111" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
-      <c r="D111" s="4"/>
+      <c r="D111" s="9"/>
       <c r="E111" s="4"/>
-      <c r="G111" s="8"/>
+      <c r="F111" s="4"/>
       <c r="H111" s="8"/>
-      <c r="J111" s="8"/>
+      <c r="I111" s="9"/>
       <c r="K111" s="8"/>
       <c r="L111" s="8"/>
       <c r="M111" s="8"/>
@@ -4498,15 +4661,16 @@
       <c r="R111" s="8"/>
       <c r="S111" s="8"/>
       <c r="T111" s="8"/>
-    </row>
-    <row r="112" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U111" s="8"/>
+    </row>
+    <row r="112" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
-      <c r="D112" s="4"/>
+      <c r="D112" s="9"/>
       <c r="E112" s="4"/>
-      <c r="G112" s="8"/>
+      <c r="F112" s="4"/>
       <c r="H112" s="8"/>
-      <c r="J112" s="8"/>
+      <c r="I112" s="9"/>
       <c r="K112" s="8"/>
       <c r="L112" s="8"/>
       <c r="M112" s="8"/>
@@ -4517,15 +4681,16 @@
       <c r="R112" s="8"/>
       <c r="S112" s="8"/>
       <c r="T112" s="8"/>
-    </row>
-    <row r="113" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U112" s="8"/>
+    </row>
+    <row r="113" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
-      <c r="D113" s="4"/>
+      <c r="D113" s="9"/>
       <c r="E113" s="4"/>
-      <c r="G113" s="8"/>
+      <c r="F113" s="4"/>
       <c r="H113" s="8"/>
-      <c r="J113" s="8"/>
+      <c r="I113" s="9"/>
       <c r="K113" s="8"/>
       <c r="L113" s="8"/>
       <c r="M113" s="8"/>
@@ -4536,15 +4701,16 @@
       <c r="R113" s="8"/>
       <c r="S113" s="8"/>
       <c r="T113" s="8"/>
-    </row>
-    <row r="114" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U113" s="8"/>
+    </row>
+    <row r="114" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
-      <c r="D114" s="4"/>
+      <c r="D114" s="9"/>
       <c r="E114" s="4"/>
-      <c r="G114" s="8"/>
+      <c r="F114" s="4"/>
       <c r="H114" s="8"/>
-      <c r="J114" s="8"/>
+      <c r="I114" s="9"/>
       <c r="K114" s="8"/>
       <c r="L114" s="8"/>
       <c r="M114" s="8"/>
@@ -4555,15 +4721,16 @@
       <c r="R114" s="8"/>
       <c r="S114" s="8"/>
       <c r="T114" s="8"/>
-    </row>
-    <row r="115" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U114" s="8"/>
+    </row>
+    <row r="115" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
-      <c r="D115" s="4"/>
+      <c r="D115" s="9"/>
       <c r="E115" s="4"/>
-      <c r="G115" s="8"/>
+      <c r="F115" s="4"/>
       <c r="H115" s="8"/>
-      <c r="J115" s="8"/>
+      <c r="I115" s="9"/>
       <c r="K115" s="8"/>
       <c r="L115" s="8"/>
       <c r="M115" s="8"/>
@@ -4574,15 +4741,16 @@
       <c r="R115" s="8"/>
       <c r="S115" s="8"/>
       <c r="T115" s="8"/>
-    </row>
-    <row r="116" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U115" s="8"/>
+    </row>
+    <row r="116" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
-      <c r="D116" s="4"/>
+      <c r="D116" s="9"/>
       <c r="E116" s="4"/>
-      <c r="G116" s="8"/>
+      <c r="F116" s="4"/>
       <c r="H116" s="8"/>
-      <c r="J116" s="8"/>
+      <c r="I116" s="9"/>
       <c r="K116" s="8"/>
       <c r="L116" s="8"/>
       <c r="M116" s="8"/>
@@ -4593,15 +4761,16 @@
       <c r="R116" s="8"/>
       <c r="S116" s="8"/>
       <c r="T116" s="8"/>
-    </row>
-    <row r="117" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U116" s="8"/>
+    </row>
+    <row r="117" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
-      <c r="D117" s="4"/>
+      <c r="D117" s="9"/>
       <c r="E117" s="4"/>
-      <c r="G117" s="8"/>
+      <c r="F117" s="4"/>
       <c r="H117" s="8"/>
-      <c r="J117" s="8"/>
+      <c r="I117" s="9"/>
       <c r="K117" s="8"/>
       <c r="L117" s="8"/>
       <c r="M117" s="8"/>
@@ -4612,15 +4781,16 @@
       <c r="R117" s="8"/>
       <c r="S117" s="8"/>
       <c r="T117" s="8"/>
-    </row>
-    <row r="118" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U117" s="8"/>
+    </row>
+    <row r="118" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
-      <c r="D118" s="4"/>
+      <c r="D118" s="9"/>
       <c r="E118" s="4"/>
-      <c r="G118" s="8"/>
+      <c r="F118" s="4"/>
       <c r="H118" s="8"/>
-      <c r="J118" s="8"/>
+      <c r="I118" s="9"/>
       <c r="K118" s="8"/>
       <c r="L118" s="8"/>
       <c r="M118" s="8"/>
@@ -4631,15 +4801,16 @@
       <c r="R118" s="8"/>
       <c r="S118" s="8"/>
       <c r="T118" s="8"/>
-    </row>
-    <row r="119" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U118" s="8"/>
+    </row>
+    <row r="119" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
-      <c r="D119" s="4"/>
+      <c r="D119" s="9"/>
       <c r="E119" s="4"/>
-      <c r="G119" s="8"/>
+      <c r="F119" s="4"/>
       <c r="H119" s="8"/>
-      <c r="J119" s="8"/>
+      <c r="I119" s="9"/>
       <c r="K119" s="8"/>
       <c r="L119" s="8"/>
       <c r="M119" s="8"/>
@@ -4650,15 +4821,16 @@
       <c r="R119" s="8"/>
       <c r="S119" s="8"/>
       <c r="T119" s="8"/>
-    </row>
-    <row r="120" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U119" s="8"/>
+    </row>
+    <row r="120" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
-      <c r="D120" s="4"/>
+      <c r="D120" s="9"/>
       <c r="E120" s="4"/>
-      <c r="G120" s="8"/>
+      <c r="F120" s="4"/>
       <c r="H120" s="8"/>
-      <c r="J120" s="8"/>
+      <c r="I120" s="9"/>
       <c r="K120" s="8"/>
       <c r="L120" s="8"/>
       <c r="M120" s="8"/>
@@ -4669,15 +4841,16 @@
       <c r="R120" s="8"/>
       <c r="S120" s="8"/>
       <c r="T120" s="8"/>
-    </row>
-    <row r="121" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U120" s="8"/>
+    </row>
+    <row r="121" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
-      <c r="D121" s="4"/>
+      <c r="D121" s="9"/>
       <c r="E121" s="4"/>
-      <c r="G121" s="8"/>
+      <c r="F121" s="4"/>
       <c r="H121" s="8"/>
-      <c r="J121" s="8"/>
+      <c r="I121" s="9"/>
       <c r="K121" s="8"/>
       <c r="L121" s="8"/>
       <c r="M121" s="8"/>
@@ -4688,15 +4861,16 @@
       <c r="R121" s="8"/>
       <c r="S121" s="8"/>
       <c r="T121" s="8"/>
-    </row>
-    <row r="122" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U121" s="8"/>
+    </row>
+    <row r="122" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
-      <c r="D122" s="4"/>
+      <c r="D122" s="9"/>
       <c r="E122" s="4"/>
-      <c r="G122" s="8"/>
+      <c r="F122" s="4"/>
       <c r="H122" s="8"/>
-      <c r="J122" s="8"/>
+      <c r="I122" s="9"/>
       <c r="K122" s="8"/>
       <c r="L122" s="8"/>
       <c r="M122" s="8"/>
@@ -4707,15 +4881,16 @@
       <c r="R122" s="8"/>
       <c r="S122" s="8"/>
       <c r="T122" s="8"/>
-    </row>
-    <row r="123" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U122" s="8"/>
+    </row>
+    <row r="123" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
-      <c r="D123" s="4"/>
+      <c r="D123" s="9"/>
       <c r="E123" s="4"/>
-      <c r="G123" s="8"/>
+      <c r="F123" s="4"/>
       <c r="H123" s="8"/>
-      <c r="J123" s="8"/>
+      <c r="I123" s="9"/>
       <c r="K123" s="8"/>
       <c r="L123" s="8"/>
       <c r="M123" s="8"/>
@@ -4726,15 +4901,16 @@
       <c r="R123" s="8"/>
       <c r="S123" s="8"/>
       <c r="T123" s="8"/>
-    </row>
-    <row r="124" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U123" s="8"/>
+    </row>
+    <row r="124" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
-      <c r="D124" s="4"/>
+      <c r="D124" s="9"/>
       <c r="E124" s="4"/>
-      <c r="G124" s="8"/>
+      <c r="F124" s="4"/>
       <c r="H124" s="8"/>
-      <c r="J124" s="8"/>
+      <c r="I124" s="9"/>
       <c r="K124" s="8"/>
       <c r="L124" s="8"/>
       <c r="M124" s="8"/>
@@ -4745,15 +4921,16 @@
       <c r="R124" s="8"/>
       <c r="S124" s="8"/>
       <c r="T124" s="8"/>
-    </row>
-    <row r="125" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U124" s="8"/>
+    </row>
+    <row r="125" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
-      <c r="D125" s="4"/>
+      <c r="D125" s="9"/>
       <c r="E125" s="4"/>
-      <c r="G125" s="8"/>
+      <c r="F125" s="4"/>
       <c r="H125" s="8"/>
-      <c r="J125" s="8"/>
+      <c r="I125" s="9"/>
       <c r="K125" s="8"/>
       <c r="L125" s="8"/>
       <c r="M125" s="8"/>
@@ -4764,15 +4941,16 @@
       <c r="R125" s="8"/>
       <c r="S125" s="8"/>
       <c r="T125" s="8"/>
-    </row>
-    <row r="126" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U125" s="8"/>
+    </row>
+    <row r="126" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
-      <c r="D126" s="4"/>
+      <c r="D126" s="9"/>
       <c r="E126" s="4"/>
-      <c r="G126" s="8"/>
+      <c r="F126" s="4"/>
       <c r="H126" s="8"/>
-      <c r="J126" s="8"/>
+      <c r="I126" s="9"/>
       <c r="K126" s="8"/>
       <c r="L126" s="8"/>
       <c r="M126" s="8"/>
@@ -4783,15 +4961,16 @@
       <c r="R126" s="8"/>
       <c r="S126" s="8"/>
       <c r="T126" s="8"/>
-    </row>
-    <row r="127" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U126" s="8"/>
+    </row>
+    <row r="127" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
-      <c r="D127" s="4"/>
+      <c r="D127" s="9"/>
       <c r="E127" s="4"/>
-      <c r="G127" s="8"/>
+      <c r="F127" s="4"/>
       <c r="H127" s="8"/>
-      <c r="J127" s="8"/>
+      <c r="I127" s="9"/>
       <c r="K127" s="8"/>
       <c r="L127" s="8"/>
       <c r="M127" s="8"/>
@@ -4802,15 +4981,16 @@
       <c r="R127" s="8"/>
       <c r="S127" s="8"/>
       <c r="T127" s="8"/>
-    </row>
-    <row r="128" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U127" s="8"/>
+    </row>
+    <row r="128" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
-      <c r="D128" s="4"/>
+      <c r="D128" s="9"/>
       <c r="E128" s="4"/>
-      <c r="G128" s="8"/>
+      <c r="F128" s="4"/>
       <c r="H128" s="8"/>
-      <c r="J128" s="8"/>
+      <c r="I128" s="9"/>
       <c r="K128" s="8"/>
       <c r="L128" s="8"/>
       <c r="M128" s="8"/>
@@ -4821,15 +5001,16 @@
       <c r="R128" s="8"/>
       <c r="S128" s="8"/>
       <c r="T128" s="8"/>
-    </row>
-    <row r="129" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U128" s="8"/>
+    </row>
+    <row r="129" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
-      <c r="D129" s="4"/>
+      <c r="D129" s="9"/>
       <c r="E129" s="4"/>
-      <c r="G129" s="8"/>
+      <c r="F129" s="4"/>
       <c r="H129" s="8"/>
-      <c r="J129" s="8"/>
+      <c r="I129" s="9"/>
       <c r="K129" s="8"/>
       <c r="L129" s="8"/>
       <c r="M129" s="8"/>
@@ -4840,15 +5021,16 @@
       <c r="R129" s="8"/>
       <c r="S129" s="8"/>
       <c r="T129" s="8"/>
-    </row>
-    <row r="130" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U129" s="8"/>
+    </row>
+    <row r="130" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
-      <c r="D130" s="4"/>
+      <c r="D130" s="9"/>
       <c r="E130" s="4"/>
-      <c r="G130" s="8"/>
+      <c r="F130" s="4"/>
       <c r="H130" s="8"/>
-      <c r="J130" s="8"/>
+      <c r="I130" s="9"/>
       <c r="K130" s="8"/>
       <c r="L130" s="8"/>
       <c r="M130" s="8"/>
@@ -4859,15 +5041,16 @@
       <c r="R130" s="8"/>
       <c r="S130" s="8"/>
       <c r="T130" s="8"/>
-    </row>
-    <row r="131" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U130" s="8"/>
+    </row>
+    <row r="131" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
-      <c r="D131" s="4"/>
+      <c r="D131" s="9"/>
       <c r="E131" s="4"/>
-      <c r="G131" s="8"/>
+      <c r="F131" s="4"/>
       <c r="H131" s="8"/>
-      <c r="J131" s="8"/>
+      <c r="I131" s="9"/>
       <c r="K131" s="8"/>
       <c r="L131" s="8"/>
       <c r="M131" s="8"/>
@@ -4878,15 +5061,16 @@
       <c r="R131" s="8"/>
       <c r="S131" s="8"/>
       <c r="T131" s="8"/>
-    </row>
-    <row r="132" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U131" s="8"/>
+    </row>
+    <row r="132" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
-      <c r="D132" s="4"/>
+      <c r="D132" s="9"/>
       <c r="E132" s="4"/>
-      <c r="G132" s="8"/>
+      <c r="F132" s="4"/>
       <c r="H132" s="8"/>
-      <c r="J132" s="8"/>
+      <c r="I132" s="9"/>
       <c r="K132" s="8"/>
       <c r="L132" s="8"/>
       <c r="M132" s="8"/>
@@ -4897,15 +5081,16 @@
       <c r="R132" s="8"/>
       <c r="S132" s="8"/>
       <c r="T132" s="8"/>
-    </row>
-    <row r="133" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U132" s="8"/>
+    </row>
+    <row r="133" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
-      <c r="D133" s="4"/>
+      <c r="D133" s="9"/>
       <c r="E133" s="4"/>
-      <c r="G133" s="8"/>
+      <c r="F133" s="4"/>
       <c r="H133" s="8"/>
-      <c r="J133" s="8"/>
+      <c r="I133" s="9"/>
       <c r="K133" s="8"/>
       <c r="L133" s="8"/>
       <c r="M133" s="8"/>
@@ -4916,15 +5101,16 @@
       <c r="R133" s="8"/>
       <c r="S133" s="8"/>
       <c r="T133" s="8"/>
-    </row>
-    <row r="134" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U133" s="8"/>
+    </row>
+    <row r="134" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
-      <c r="D134" s="4"/>
+      <c r="D134" s="9"/>
       <c r="E134" s="4"/>
-      <c r="G134" s="8"/>
+      <c r="F134" s="4"/>
       <c r="H134" s="8"/>
-      <c r="J134" s="8"/>
+      <c r="I134" s="9"/>
       <c r="K134" s="8"/>
       <c r="L134" s="8"/>
       <c r="M134" s="8"/>
@@ -4935,15 +5121,16 @@
       <c r="R134" s="8"/>
       <c r="S134" s="8"/>
       <c r="T134" s="8"/>
-    </row>
-    <row r="135" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U134" s="8"/>
+    </row>
+    <row r="135" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
-      <c r="D135" s="4"/>
+      <c r="D135" s="9"/>
       <c r="E135" s="4"/>
-      <c r="G135" s="8"/>
+      <c r="F135" s="4"/>
       <c r="H135" s="8"/>
-      <c r="J135" s="8"/>
+      <c r="I135" s="9"/>
       <c r="K135" s="8"/>
       <c r="L135" s="8"/>
       <c r="M135" s="8"/>
@@ -4954,15 +5141,16 @@
       <c r="R135" s="8"/>
       <c r="S135" s="8"/>
       <c r="T135" s="8"/>
-    </row>
-    <row r="136" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U135" s="8"/>
+    </row>
+    <row r="136" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
-      <c r="D136" s="4"/>
+      <c r="D136" s="9"/>
       <c r="E136" s="4"/>
-      <c r="G136" s="8"/>
+      <c r="F136" s="4"/>
       <c r="H136" s="8"/>
-      <c r="J136" s="8"/>
+      <c r="I136" s="9"/>
       <c r="K136" s="8"/>
       <c r="L136" s="8"/>
       <c r="M136" s="8"/>
@@ -4973,15 +5161,16 @@
       <c r="R136" s="8"/>
       <c r="S136" s="8"/>
       <c r="T136" s="8"/>
-    </row>
-    <row r="137" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U136" s="8"/>
+    </row>
+    <row r="137" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
-      <c r="D137" s="4"/>
+      <c r="D137" s="9"/>
       <c r="E137" s="4"/>
-      <c r="G137" s="8"/>
+      <c r="F137" s="4"/>
       <c r="H137" s="8"/>
-      <c r="J137" s="8"/>
+      <c r="I137" s="9"/>
       <c r="K137" s="8"/>
       <c r="L137" s="8"/>
       <c r="M137" s="8"/>
@@ -4992,15 +5181,16 @@
       <c r="R137" s="8"/>
       <c r="S137" s="8"/>
       <c r="T137" s="8"/>
-    </row>
-    <row r="138" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U137" s="8"/>
+    </row>
+    <row r="138" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
-      <c r="D138" s="4"/>
+      <c r="D138" s="9"/>
       <c r="E138" s="4"/>
-      <c r="G138" s="8"/>
+      <c r="F138" s="4"/>
       <c r="H138" s="8"/>
-      <c r="J138" s="8"/>
+      <c r="I138" s="9"/>
       <c r="K138" s="8"/>
       <c r="L138" s="8"/>
       <c r="M138" s="8"/>
@@ -5011,15 +5201,16 @@
       <c r="R138" s="8"/>
       <c r="S138" s="8"/>
       <c r="T138" s="8"/>
-    </row>
-    <row r="139" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U138" s="8"/>
+    </row>
+    <row r="139" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
-      <c r="D139" s="4"/>
+      <c r="D139" s="9"/>
       <c r="E139" s="4"/>
-      <c r="G139" s="8"/>
+      <c r="F139" s="4"/>
       <c r="H139" s="8"/>
-      <c r="J139" s="8"/>
+      <c r="I139" s="9"/>
       <c r="K139" s="8"/>
       <c r="L139" s="8"/>
       <c r="M139" s="8"/>
@@ -5030,15 +5221,16 @@
       <c r="R139" s="8"/>
       <c r="S139" s="8"/>
       <c r="T139" s="8"/>
-    </row>
-    <row r="140" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U139" s="8"/>
+    </row>
+    <row r="140" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
-      <c r="D140" s="4"/>
+      <c r="D140" s="9"/>
       <c r="E140" s="4"/>
-      <c r="G140" s="8"/>
+      <c r="F140" s="4"/>
       <c r="H140" s="8"/>
-      <c r="J140" s="8"/>
+      <c r="I140" s="9"/>
       <c r="K140" s="8"/>
       <c r="L140" s="8"/>
       <c r="M140" s="8"/>
@@ -5049,15 +5241,16 @@
       <c r="R140" s="8"/>
       <c r="S140" s="8"/>
       <c r="T140" s="8"/>
-    </row>
-    <row r="141" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U140" s="8"/>
+    </row>
+    <row r="141" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
-      <c r="D141" s="4"/>
+      <c r="D141" s="9"/>
       <c r="E141" s="4"/>
-      <c r="G141" s="8"/>
+      <c r="F141" s="4"/>
       <c r="H141" s="8"/>
-      <c r="J141" s="8"/>
+      <c r="I141" s="9"/>
       <c r="K141" s="8"/>
       <c r="L141" s="8"/>
       <c r="M141" s="8"/>
@@ -5068,15 +5261,16 @@
       <c r="R141" s="8"/>
       <c r="S141" s="8"/>
       <c r="T141" s="8"/>
-    </row>
-    <row r="142" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U141" s="8"/>
+    </row>
+    <row r="142" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
-      <c r="D142" s="4"/>
+      <c r="D142" s="9"/>
       <c r="E142" s="4"/>
-      <c r="G142" s="8"/>
+      <c r="F142" s="4"/>
       <c r="H142" s="8"/>
-      <c r="J142" s="8"/>
+      <c r="I142" s="9"/>
       <c r="K142" s="8"/>
       <c r="L142" s="8"/>
       <c r="M142" s="8"/>
@@ -5087,15 +5281,16 @@
       <c r="R142" s="8"/>
       <c r="S142" s="8"/>
       <c r="T142" s="8"/>
-    </row>
-    <row r="143" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U142" s="8"/>
+    </row>
+    <row r="143" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
-      <c r="D143" s="4"/>
+      <c r="D143" s="9"/>
       <c r="E143" s="4"/>
-      <c r="G143" s="8"/>
+      <c r="F143" s="4"/>
       <c r="H143" s="8"/>
-      <c r="J143" s="8"/>
+      <c r="I143" s="9"/>
       <c r="K143" s="8"/>
       <c r="L143" s="8"/>
       <c r="M143" s="8"/>
@@ -5106,15 +5301,16 @@
       <c r="R143" s="8"/>
       <c r="S143" s="8"/>
       <c r="T143" s="8"/>
-    </row>
-    <row r="144" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U143" s="8"/>
+    </row>
+    <row r="144" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
-      <c r="D144" s="4"/>
+      <c r="D144" s="9"/>
       <c r="E144" s="4"/>
-      <c r="G144" s="8"/>
+      <c r="F144" s="4"/>
       <c r="H144" s="8"/>
-      <c r="J144" s="8"/>
+      <c r="I144" s="9"/>
       <c r="K144" s="8"/>
       <c r="L144" s="8"/>
       <c r="M144" s="8"/>
@@ -5125,15 +5321,16 @@
       <c r="R144" s="8"/>
       <c r="S144" s="8"/>
       <c r="T144" s="8"/>
-    </row>
-    <row r="145" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U144" s="8"/>
+    </row>
+    <row r="145" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
-      <c r="D145" s="4"/>
+      <c r="D145" s="9"/>
       <c r="E145" s="4"/>
-      <c r="G145" s="8"/>
+      <c r="F145" s="4"/>
       <c r="H145" s="8"/>
-      <c r="J145" s="8"/>
+      <c r="I145" s="9"/>
       <c r="K145" s="8"/>
       <c r="L145" s="8"/>
       <c r="M145" s="8"/>
@@ -5144,15 +5341,16 @@
       <c r="R145" s="8"/>
       <c r="S145" s="8"/>
       <c r="T145" s="8"/>
-    </row>
-    <row r="146" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U145" s="8"/>
+    </row>
+    <row r="146" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
-      <c r="D146" s="4"/>
+      <c r="D146" s="9"/>
       <c r="E146" s="4"/>
-      <c r="G146" s="8"/>
+      <c r="F146" s="4"/>
       <c r="H146" s="8"/>
-      <c r="J146" s="8"/>
+      <c r="I146" s="9"/>
       <c r="K146" s="8"/>
       <c r="L146" s="8"/>
       <c r="M146" s="8"/>
@@ -5163,15 +5361,16 @@
       <c r="R146" s="8"/>
       <c r="S146" s="8"/>
       <c r="T146" s="8"/>
-    </row>
-    <row r="147" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U146" s="8"/>
+    </row>
+    <row r="147" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
-      <c r="D147" s="4"/>
+      <c r="D147" s="9"/>
       <c r="E147" s="4"/>
-      <c r="G147" s="8"/>
+      <c r="F147" s="4"/>
       <c r="H147" s="8"/>
-      <c r="J147" s="8"/>
+      <c r="I147" s="9"/>
       <c r="K147" s="8"/>
       <c r="L147" s="8"/>
       <c r="M147" s="8"/>
@@ -5182,15 +5381,16 @@
       <c r="R147" s="8"/>
       <c r="S147" s="8"/>
       <c r="T147" s="8"/>
-    </row>
-    <row r="148" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U147" s="8"/>
+    </row>
+    <row r="148" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
-      <c r="D148" s="4"/>
+      <c r="D148" s="9"/>
       <c r="E148" s="4"/>
-      <c r="G148" s="8"/>
+      <c r="F148" s="4"/>
       <c r="H148" s="8"/>
-      <c r="J148" s="8"/>
+      <c r="I148" s="9"/>
       <c r="K148" s="8"/>
       <c r="L148" s="8"/>
       <c r="M148" s="8"/>
@@ -5201,15 +5401,16 @@
       <c r="R148" s="8"/>
       <c r="S148" s="8"/>
       <c r="T148" s="8"/>
-    </row>
-    <row r="149" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U148" s="8"/>
+    </row>
+    <row r="149" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
-      <c r="D149" s="4"/>
+      <c r="D149" s="9"/>
       <c r="E149" s="4"/>
-      <c r="G149" s="8"/>
+      <c r="F149" s="4"/>
       <c r="H149" s="8"/>
-      <c r="J149" s="8"/>
+      <c r="I149" s="9"/>
       <c r="K149" s="8"/>
       <c r="L149" s="8"/>
       <c r="M149" s="8"/>
@@ -5220,15 +5421,16 @@
       <c r="R149" s="8"/>
       <c r="S149" s="8"/>
       <c r="T149" s="8"/>
-    </row>
-    <row r="150" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U149" s="8"/>
+    </row>
+    <row r="150" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
-      <c r="D150" s="4"/>
+      <c r="D150" s="9"/>
       <c r="E150" s="4"/>
-      <c r="G150" s="8"/>
+      <c r="F150" s="4"/>
       <c r="H150" s="8"/>
-      <c r="J150" s="8"/>
+      <c r="I150" s="9"/>
       <c r="K150" s="8"/>
       <c r="L150" s="8"/>
       <c r="M150" s="8"/>
@@ -5239,15 +5441,16 @@
       <c r="R150" s="8"/>
       <c r="S150" s="8"/>
       <c r="T150" s="8"/>
-    </row>
-    <row r="151" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U150" s="8"/>
+    </row>
+    <row r="151" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
-      <c r="D151" s="4"/>
+      <c r="D151" s="9"/>
       <c r="E151" s="4"/>
-      <c r="G151" s="8"/>
+      <c r="F151" s="4"/>
       <c r="H151" s="8"/>
-      <c r="J151" s="8"/>
+      <c r="I151" s="9"/>
       <c r="K151" s="8"/>
       <c r="L151" s="8"/>
       <c r="M151" s="8"/>
@@ -5258,15 +5461,16 @@
       <c r="R151" s="8"/>
       <c r="S151" s="8"/>
       <c r="T151" s="8"/>
-    </row>
-    <row r="152" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U151" s="8"/>
+    </row>
+    <row r="152" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
-      <c r="D152" s="4"/>
+      <c r="D152" s="9"/>
       <c r="E152" s="4"/>
-      <c r="G152" s="8"/>
+      <c r="F152" s="4"/>
       <c r="H152" s="8"/>
-      <c r="J152" s="8"/>
+      <c r="I152" s="9"/>
       <c r="K152" s="8"/>
       <c r="L152" s="8"/>
       <c r="M152" s="8"/>
@@ -5277,15 +5481,16 @@
       <c r="R152" s="8"/>
       <c r="S152" s="8"/>
       <c r="T152" s="8"/>
-    </row>
-    <row r="153" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U152" s="8"/>
+    </row>
+    <row r="153" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
-      <c r="D153" s="4"/>
+      <c r="D153" s="9"/>
       <c r="E153" s="4"/>
-      <c r="G153" s="8"/>
+      <c r="F153" s="4"/>
       <c r="H153" s="8"/>
-      <c r="J153" s="8"/>
+      <c r="I153" s="9"/>
       <c r="K153" s="8"/>
       <c r="L153" s="8"/>
       <c r="M153" s="8"/>
@@ -5296,15 +5501,16 @@
       <c r="R153" s="8"/>
       <c r="S153" s="8"/>
       <c r="T153" s="8"/>
-    </row>
-    <row r="154" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U153" s="8"/>
+    </row>
+    <row r="154" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
-      <c r="D154" s="4"/>
+      <c r="D154" s="9"/>
       <c r="E154" s="4"/>
-      <c r="G154" s="8"/>
+      <c r="F154" s="4"/>
       <c r="H154" s="8"/>
-      <c r="J154" s="8"/>
+      <c r="I154" s="9"/>
       <c r="K154" s="8"/>
       <c r="L154" s="8"/>
       <c r="M154" s="8"/>
@@ -5315,15 +5521,16 @@
       <c r="R154" s="8"/>
       <c r="S154" s="8"/>
       <c r="T154" s="8"/>
-    </row>
-    <row r="155" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U154" s="8"/>
+    </row>
+    <row r="155" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
-      <c r="D155" s="4"/>
+      <c r="D155" s="9"/>
       <c r="E155" s="4"/>
-      <c r="G155" s="8"/>
+      <c r="F155" s="4"/>
       <c r="H155" s="8"/>
-      <c r="J155" s="8"/>
+      <c r="I155" s="9"/>
       <c r="K155" s="8"/>
       <c r="L155" s="8"/>
       <c r="M155" s="8"/>
@@ -5334,15 +5541,16 @@
       <c r="R155" s="8"/>
       <c r="S155" s="8"/>
       <c r="T155" s="8"/>
-    </row>
-    <row r="156" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U155" s="8"/>
+    </row>
+    <row r="156" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
-      <c r="D156" s="4"/>
+      <c r="D156" s="9"/>
       <c r="E156" s="4"/>
-      <c r="G156" s="8"/>
+      <c r="F156" s="4"/>
       <c r="H156" s="8"/>
-      <c r="J156" s="8"/>
+      <c r="I156" s="9"/>
       <c r="K156" s="8"/>
       <c r="L156" s="8"/>
       <c r="M156" s="8"/>
@@ -5353,15 +5561,16 @@
       <c r="R156" s="8"/>
       <c r="S156" s="8"/>
       <c r="T156" s="8"/>
-    </row>
-    <row r="157" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U156" s="8"/>
+    </row>
+    <row r="157" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
-      <c r="D157" s="4"/>
+      <c r="D157" s="9"/>
       <c r="E157" s="4"/>
-      <c r="G157" s="8"/>
+      <c r="F157" s="4"/>
       <c r="H157" s="8"/>
-      <c r="J157" s="8"/>
+      <c r="I157" s="9"/>
       <c r="K157" s="8"/>
       <c r="L157" s="8"/>
       <c r="M157" s="8"/>
@@ -5372,15 +5581,16 @@
       <c r="R157" s="8"/>
       <c r="S157" s="8"/>
       <c r="T157" s="8"/>
-    </row>
-    <row r="158" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U157" s="8"/>
+    </row>
+    <row r="158" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
-      <c r="D158" s="4"/>
+      <c r="D158" s="9"/>
       <c r="E158" s="4"/>
-      <c r="G158" s="8"/>
+      <c r="F158" s="4"/>
       <c r="H158" s="8"/>
-      <c r="J158" s="8"/>
+      <c r="I158" s="9"/>
       <c r="K158" s="8"/>
       <c r="L158" s="8"/>
       <c r="M158" s="8"/>
@@ -5391,15 +5601,16 @@
       <c r="R158" s="8"/>
       <c r="S158" s="8"/>
       <c r="T158" s="8"/>
-    </row>
-    <row r="159" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U158" s="8"/>
+    </row>
+    <row r="159" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
-      <c r="D159" s="4"/>
+      <c r="D159" s="9"/>
       <c r="E159" s="4"/>
-      <c r="G159" s="8"/>
+      <c r="F159" s="4"/>
       <c r="H159" s="8"/>
-      <c r="J159" s="8"/>
+      <c r="I159" s="9"/>
       <c r="K159" s="8"/>
       <c r="L159" s="8"/>
       <c r="M159" s="8"/>
@@ -5410,372 +5621,454 @@
       <c r="R159" s="8"/>
       <c r="S159" s="8"/>
       <c r="T159" s="8"/>
-    </row>
-    <row r="160" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U159" s="8"/>
+    </row>
+    <row r="160" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
-      <c r="D160" s="4"/>
+      <c r="D160" s="9"/>
       <c r="E160" s="4"/>
-    </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F160" s="4"/>
+      <c r="H160" s="8"/>
+      <c r="I160" s="9"/>
+      <c r="K160" s="8"/>
+      <c r="L160" s="8"/>
+      <c r="M160" s="8"/>
+      <c r="N160" s="8"/>
+      <c r="O160" s="8"/>
+      <c r="P160" s="8"/>
+      <c r="Q160" s="8"/>
+      <c r="R160" s="8"/>
+      <c r="S160" s="8"/>
+      <c r="T160" s="8"/>
+      <c r="U160" s="8"/>
+    </row>
+    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
-      <c r="D161" s="4"/>
+      <c r="D161" s="9"/>
       <c r="E161" s="4"/>
-    </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F161" s="4"/>
+    </row>
+    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
-      <c r="D162" s="4"/>
+      <c r="D162" s="9"/>
       <c r="E162" s="4"/>
-    </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F162" s="4"/>
+    </row>
+    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
-      <c r="D163" s="4"/>
+      <c r="D163" s="9"/>
       <c r="E163" s="4"/>
-    </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F163" s="4"/>
+    </row>
+    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
-      <c r="D164" s="4"/>
+      <c r="D164" s="9"/>
       <c r="E164" s="4"/>
-    </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F164" s="4"/>
+    </row>
+    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
-      <c r="D165" s="4"/>
+      <c r="D165" s="9"/>
       <c r="E165" s="4"/>
-    </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F165" s="4"/>
+    </row>
+    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
-      <c r="D166" s="4"/>
+      <c r="D166" s="9"/>
       <c r="E166" s="4"/>
-    </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F166" s="4"/>
+    </row>
+    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
-      <c r="D167" s="4"/>
+      <c r="D167" s="9"/>
       <c r="E167" s="4"/>
-    </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F167" s="4"/>
+    </row>
+    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
-      <c r="D168" s="4"/>
+      <c r="D168" s="9"/>
       <c r="E168" s="4"/>
-    </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F168" s="4"/>
+    </row>
+    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
-      <c r="D169" s="4"/>
+      <c r="D169" s="9"/>
       <c r="E169" s="4"/>
-    </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F169" s="4"/>
+    </row>
+    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
-      <c r="D170" s="4"/>
+      <c r="D170" s="9"/>
       <c r="E170" s="4"/>
-    </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F170" s="4"/>
+    </row>
+    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
-      <c r="D171" s="4"/>
+      <c r="D171" s="9"/>
       <c r="E171" s="4"/>
-    </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F171" s="4"/>
+    </row>
+    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
-      <c r="D172" s="4"/>
+      <c r="D172" s="9"/>
       <c r="E172" s="4"/>
-    </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F172" s="4"/>
+    </row>
+    <row r="173" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
-      <c r="D173" s="4"/>
+      <c r="D173" s="9"/>
       <c r="E173" s="4"/>
-    </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F173" s="4"/>
+    </row>
+    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
-      <c r="D174" s="4"/>
+      <c r="D174" s="9"/>
       <c r="E174" s="4"/>
-    </row>
-    <row r="175" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F174" s="4"/>
+    </row>
+    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
-      <c r="D175" s="4"/>
+      <c r="D175" s="9"/>
       <c r="E175" s="4"/>
-    </row>
-    <row r="176" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F175" s="4"/>
+    </row>
+    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
-      <c r="D176" s="4"/>
+      <c r="D176" s="9"/>
       <c r="E176" s="4"/>
-    </row>
-    <row r="177" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F176" s="4"/>
+    </row>
+    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
-      <c r="D177" s="4"/>
+      <c r="D177" s="9"/>
       <c r="E177" s="4"/>
-    </row>
-    <row r="178" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F177" s="4"/>
+    </row>
+    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
-      <c r="D178" s="4"/>
+      <c r="D178" s="9"/>
       <c r="E178" s="4"/>
-    </row>
-    <row r="179" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F178" s="4"/>
+    </row>
+    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
-      <c r="D179" s="4"/>
+      <c r="D179" s="9"/>
       <c r="E179" s="4"/>
-    </row>
-    <row r="180" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F179" s="4"/>
+    </row>
+    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
-      <c r="D180" s="4"/>
+      <c r="D180" s="9"/>
       <c r="E180" s="4"/>
-    </row>
-    <row r="181" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F180" s="4"/>
+    </row>
+    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
-      <c r="D181" s="4"/>
+      <c r="D181" s="9"/>
       <c r="E181" s="4"/>
-    </row>
-    <row r="182" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F181" s="4"/>
+    </row>
+    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
-      <c r="D182" s="4"/>
+      <c r="D182" s="9"/>
       <c r="E182" s="4"/>
-    </row>
-    <row r="183" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F182" s="4"/>
+    </row>
+    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
-      <c r="D183" s="4"/>
+      <c r="D183" s="9"/>
       <c r="E183" s="4"/>
-    </row>
-    <row r="184" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F183" s="4"/>
+    </row>
+    <row r="184" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
-      <c r="D184" s="4"/>
+      <c r="D184" s="9"/>
       <c r="E184" s="4"/>
-    </row>
-    <row r="185" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F184" s="4"/>
+    </row>
+    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
-      <c r="D185" s="4"/>
+      <c r="D185" s="9"/>
       <c r="E185" s="4"/>
-    </row>
-    <row r="186" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F185" s="4"/>
+    </row>
+    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B186" s="8"/>
       <c r="C186" s="8"/>
-      <c r="D186" s="4"/>
+      <c r="D186" s="9"/>
       <c r="E186" s="4"/>
-    </row>
-    <row r="187" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F186" s="4"/>
+    </row>
+    <row r="187" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
-      <c r="D187" s="4"/>
+      <c r="D187" s="9"/>
       <c r="E187" s="4"/>
-    </row>
-    <row r="188" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F187" s="4"/>
+    </row>
+    <row r="188" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
-      <c r="D188" s="4"/>
+      <c r="D188" s="9"/>
       <c r="E188" s="4"/>
-    </row>
-    <row r="189" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F188" s="4"/>
+    </row>
+    <row r="189" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
-      <c r="D189" s="4"/>
+      <c r="D189" s="9"/>
       <c r="E189" s="4"/>
-    </row>
-    <row r="190" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F189" s="4"/>
+    </row>
+    <row r="190" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
-      <c r="D190" s="4"/>
+      <c r="D190" s="9"/>
       <c r="E190" s="4"/>
-    </row>
-    <row r="191" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F190" s="4"/>
+    </row>
+    <row r="191" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
-      <c r="D191" s="4"/>
+      <c r="D191" s="9"/>
       <c r="E191" s="4"/>
-    </row>
-    <row r="192" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F191" s="4"/>
+    </row>
+    <row r="192" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
-      <c r="D192" s="4"/>
+      <c r="D192" s="9"/>
       <c r="E192" s="4"/>
-    </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F192" s="4"/>
+    </row>
+    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
-      <c r="D193" s="4"/>
+      <c r="D193" s="9"/>
       <c r="E193" s="4"/>
-    </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F193" s="4"/>
+    </row>
+    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
-      <c r="D194" s="4"/>
+      <c r="D194" s="9"/>
       <c r="E194" s="4"/>
-    </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F194" s="4"/>
+    </row>
+    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B195" s="8"/>
       <c r="C195" s="8"/>
-      <c r="D195" s="4"/>
+      <c r="D195" s="9"/>
       <c r="E195" s="4"/>
-    </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F195" s="4"/>
+    </row>
+    <row r="196" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B196" s="8"/>
       <c r="C196" s="8"/>
-      <c r="D196" s="4"/>
+      <c r="D196" s="9"/>
       <c r="E196" s="4"/>
-    </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F196" s="4"/>
+    </row>
+    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B197" s="8"/>
       <c r="C197" s="8"/>
-      <c r="D197" s="4"/>
+      <c r="D197" s="9"/>
       <c r="E197" s="4"/>
-    </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F197" s="4"/>
+    </row>
+    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B198" s="8"/>
       <c r="C198" s="8"/>
-      <c r="D198" s="4"/>
+      <c r="D198" s="9"/>
       <c r="E198" s="4"/>
-    </row>
-    <row r="199" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F198" s="4"/>
+    </row>
+    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B199" s="8"/>
       <c r="C199" s="8"/>
-      <c r="D199" s="4"/>
+      <c r="D199" s="9"/>
       <c r="E199" s="4"/>
-    </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F199" s="4"/>
+    </row>
+    <row r="200" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B200" s="8"/>
       <c r="C200" s="8"/>
-      <c r="D200" s="4"/>
+      <c r="D200" s="9"/>
       <c r="E200" s="4"/>
-    </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F200" s="4"/>
+    </row>
+    <row r="201" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B201" s="8"/>
       <c r="C201" s="8"/>
-      <c r="D201" s="4"/>
+      <c r="D201" s="9"/>
       <c r="E201" s="4"/>
-    </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F201" s="4"/>
+    </row>
+    <row r="202" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B202" s="8"/>
       <c r="C202" s="8"/>
-      <c r="D202" s="4"/>
+      <c r="D202" s="9"/>
       <c r="E202" s="4"/>
-    </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F202" s="4"/>
+    </row>
+    <row r="203" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B203" s="8"/>
       <c r="C203" s="8"/>
-      <c r="D203" s="4"/>
+      <c r="D203" s="9"/>
       <c r="E203" s="4"/>
-    </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F203" s="4"/>
+    </row>
+    <row r="204" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B204" s="8"/>
       <c r="C204" s="8"/>
-      <c r="D204" s="4"/>
+      <c r="D204" s="9"/>
       <c r="E204" s="4"/>
-    </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F204" s="4"/>
+    </row>
+    <row r="205" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B205" s="8"/>
       <c r="C205" s="8"/>
-      <c r="D205" s="4"/>
+      <c r="D205" s="9"/>
       <c r="E205" s="4"/>
-    </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F205" s="4"/>
+    </row>
+    <row r="206" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B206" s="8"/>
       <c r="C206" s="8"/>
-      <c r="D206" s="4"/>
+      <c r="D206" s="9"/>
       <c r="E206" s="4"/>
-    </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F206" s="4"/>
+    </row>
+    <row r="207" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B207" s="8"/>
       <c r="C207" s="8"/>
-      <c r="D207" s="4"/>
+      <c r="D207" s="9"/>
       <c r="E207" s="4"/>
-    </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F207" s="4"/>
+    </row>
+    <row r="208" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B208" s="8"/>
       <c r="C208" s="8"/>
-      <c r="D208" s="4"/>
+      <c r="D208" s="9"/>
       <c r="E208" s="4"/>
-    </row>
-    <row r="209" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F208" s="4"/>
+    </row>
+    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B209" s="8"/>
       <c r="C209" s="8"/>
-      <c r="D209" s="4"/>
+      <c r="D209" s="9"/>
       <c r="E209" s="4"/>
-    </row>
-    <row r="210" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F209" s="4"/>
+    </row>
+    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B210" s="8"/>
       <c r="C210" s="8"/>
-      <c r="D210" s="4"/>
+      <c r="D210" s="9"/>
       <c r="E210" s="4"/>
-    </row>
-    <row r="211" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F210" s="4"/>
+    </row>
+    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B211" s="8"/>
       <c r="C211" s="8"/>
-      <c r="D211" s="4"/>
+      <c r="D211" s="9"/>
       <c r="E211" s="4"/>
-    </row>
-    <row r="212" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F211" s="4"/>
+    </row>
+    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B212" s="8"/>
       <c r="C212" s="8"/>
-      <c r="D212" s="4"/>
+      <c r="D212" s="9"/>
       <c r="E212" s="4"/>
-    </row>
-    <row r="213" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F212" s="4"/>
+    </row>
+    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B213" s="8"/>
       <c r="C213" s="8"/>
-      <c r="D213" s="4"/>
+      <c r="D213" s="9"/>
       <c r="E213" s="4"/>
-    </row>
-    <row r="214" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F213" s="4"/>
+    </row>
+    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B214" s="8"/>
       <c r="C214" s="8"/>
-      <c r="D214" s="4"/>
+      <c r="D214" s="9"/>
       <c r="E214" s="4"/>
-    </row>
-    <row r="215" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F214" s="4"/>
+    </row>
+    <row r="215" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B215" s="8"/>
       <c r="C215" s="8"/>
-      <c r="D215" s="4"/>
+      <c r="D215" s="9"/>
       <c r="E215" s="4"/>
-    </row>
-    <row r="216" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F215" s="4"/>
+    </row>
+    <row r="216" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B216" s="8"/>
       <c r="C216" s="8"/>
-      <c r="D216" s="4"/>
+      <c r="D216" s="9"/>
       <c r="E216" s="4"/>
-    </row>
-    <row r="217" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F216" s="4"/>
+    </row>
+    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B217" s="8"/>
       <c r="C217" s="8"/>
-      <c r="D217" s="4"/>
+      <c r="D217" s="9"/>
       <c r="E217" s="4"/>
-    </row>
-    <row r="218" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F217" s="4"/>
+    </row>
+    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B218" s="8"/>
       <c r="C218" s="8"/>
-      <c r="D218" s="4"/>
+      <c r="D218" s="9"/>
       <c r="E218" s="4"/>
-    </row>
-    <row r="219" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F218" s="4"/>
+    </row>
+    <row r="219" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B219" s="8"/>
       <c r="C219" s="8"/>
-      <c r="D219" s="4"/>
+      <c r="D219" s="9"/>
       <c r="E219" s="4"/>
-    </row>
-    <row r="220" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F219" s="4"/>
+    </row>
+    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B220" s="8"/>
       <c r="C220" s="8"/>
-      <c r="D220" s="4"/>
+      <c r="D220" s="9"/>
       <c r="E220" s="4"/>
+      <c r="F220" s="4"/>
+    </row>
+    <row r="221" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B221" s="8"/>
+      <c r="C221" s="8"/>
+      <c r="D221" s="9"/>
+      <c r="E221" s="4"/>
+      <c r="F221" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
This is probably the last commit in this repository. Thanks for everything!
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46B6B29-A6AF-4973-9E47-A80CF98CE1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB710E89-6A38-4017-88A9-3625451DE781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="План" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="259">
   <si>
     <t>Модуль для торговли через эмуляцию нажатий мыши и клавиш</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Торговля по лимитам разных таймфремов с применением полос Боллинджера</t>
   </si>
   <si>
-    <t>Действует</t>
-  </si>
-  <si>
     <t>Редкие сделки, небольшая прибыль. Пропуск основных движений. Но в целом бот работает в плюс</t>
   </si>
   <si>
@@ -533,9 +530,6 @@
     <t>Упрощенный выход в PTA2</t>
   </si>
   <si>
-    <t>Тест</t>
-  </si>
-  <si>
     <t>PTA3_ADCC</t>
   </si>
   <si>
@@ -807,6 +801,12 @@
   </si>
   <si>
     <t>Использует данные с APIMOEX и стратегии из RL</t>
+  </si>
+  <si>
+    <t>Абстрак-5</t>
+  </si>
+  <si>
+    <t>Абстракный бот для стратегий RL. Проект переехал в RL</t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -918,9 +918,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -1719,7 +1716,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2754,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2775,7 +2772,7 @@
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F1" s="12">
         <f ca="1">NOW()</f>
-        <v>45735.684422106482</v>
+        <v>45741.044833217595</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -3296,7 +3293,7 @@
         <v>30</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J14" s="14">
         <v>5.4</v>
@@ -3318,13 +3315,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="8">
         <v>5</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E15" s="10">
         <v>45505</v>
@@ -3340,7 +3337,7 @@
         <v>30</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J15" s="14">
         <v>5.7</v>
@@ -3362,13 +3359,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="8">
         <v>5</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" s="10">
         <v>45515</v>
@@ -3384,7 +3381,7 @@
         <v>30</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J16" s="14">
         <v>4.9000000000000004</v>
@@ -3406,13 +3403,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="8">
         <v>5</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="10">
         <v>45508</v>
@@ -3428,7 +3425,7 @@
         <v>30</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J17" s="14">
         <v>4.4000000000000004</v>
@@ -3450,13 +3447,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="8">
         <v>5</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="10">
         <v>45509</v>
@@ -3472,7 +3469,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J18" s="14">
         <v>5.5</v>
@@ -3494,13 +3491,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="8">
         <v>5</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" s="10">
         <v>45509</v>
@@ -3516,7 +3513,7 @@
         <v>30</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J19" s="14">
         <v>5.5</v>
@@ -3538,13 +3535,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="8">
         <v>5</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" s="10">
         <v>45509</v>
@@ -3560,7 +3557,7 @@
         <v>30</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J20" s="14">
         <v>5.6</v>
@@ -3582,13 +3579,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="8">
         <v>5</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" s="10">
         <v>45509</v>
@@ -3604,13 +3601,13 @@
         <v>30</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J21" s="14">
         <v>4.8</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
@@ -3628,13 +3625,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22" s="8">
         <v>5</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" s="10">
         <v>45510</v>
@@ -3650,7 +3647,7 @@
         <v>30</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J22" s="14">
         <v>5</v>
@@ -3672,13 +3669,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="8">
         <v>5</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" s="10">
         <v>45510</v>
@@ -3714,13 +3711,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="8">
         <v>5</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E24" s="10">
         <v>45513</v>
@@ -3736,7 +3733,7 @@
         <v>30</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J24" s="14">
         <v>4.3</v>
@@ -3758,13 +3755,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="8">
         <v>5</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E25" s="10">
         <v>45514</v>
@@ -3780,13 +3777,13 @@
         <v>30</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J25" s="14">
         <v>4.4000000000000004</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
@@ -3804,13 +3801,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="8">
         <v>5</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E26" s="10">
         <v>45514</v>
@@ -3826,7 +3823,7 @@
         <v>30</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J26" s="14">
         <v>5</v>
@@ -3848,13 +3845,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" s="8">
         <v>5</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E27" s="10">
         <v>45514</v>
@@ -3870,13 +3867,13 @@
         <v>30</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J27" s="14">
         <v>5.0999999999999996</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
@@ -3894,13 +3891,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" s="8">
         <v>5</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28" s="10">
         <v>45515</v>
@@ -3938,13 +3935,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29" s="8">
         <v>5</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E29" s="10">
         <v>45515</v>
@@ -3960,7 +3957,7 @@
         <v>30</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J29" s="14">
         <v>4.5</v>
@@ -3982,13 +3979,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30" s="8">
         <v>5</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E30" s="10">
         <v>45515</v>
@@ -4004,13 +4001,13 @@
         <v>30</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J30" s="14">
         <v>4.7</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
@@ -4028,13 +4025,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31" s="8">
         <v>5</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E31" s="10">
         <v>45516</v>
@@ -4050,7 +4047,7 @@
         <v>30</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J31" s="14">
         <v>5.0999999999999996</v>
@@ -4072,13 +4069,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C32" s="8">
         <v>5</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E32" s="10">
         <v>45516</v>
@@ -4094,13 +4091,13 @@
         <v>30</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J32" s="14">
         <v>3.4</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
@@ -4118,13 +4115,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C33" s="8">
         <v>5</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E33" s="10">
         <v>45535</v>
@@ -4140,7 +4137,7 @@
         <v>30</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J33" s="14">
         <v>3.6</v>
@@ -4162,13 +4159,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C34" s="8">
         <v>5</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E34" s="10">
         <v>45535</v>
@@ -4204,13 +4201,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C35" s="8">
         <v>5</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E35" s="10">
         <v>45535</v>
@@ -4226,10 +4223,10 @@
         <v>30</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
@@ -4247,13 +4244,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C36" s="8">
         <v>5</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E36" s="10">
         <v>45536</v>
@@ -4269,10 +4266,10 @@
         <v>30</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
@@ -4290,13 +4287,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C37" s="8">
         <v>5</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E37" s="10">
         <v>45537</v>
@@ -4312,13 +4309,13 @@
         <v>30</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J37" s="4">
         <v>4.7</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
@@ -4336,13 +4333,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C38" s="8">
         <v>5</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E38" s="10">
         <v>45537</v>
@@ -4358,13 +4355,13 @@
         <v>30</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J38" s="4">
         <v>4.5999999999999996</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
@@ -4382,13 +4379,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C39" s="8">
         <v>5</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E39" s="10">
         <v>45537</v>
@@ -4404,13 +4401,13 @@
         <v>30</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J39" s="4">
         <v>4.5999999999999996</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
@@ -4428,13 +4425,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C40" s="8">
         <v>2</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E40" s="10">
         <v>45539</v>
@@ -4467,24 +4464,26 @@
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C41" s="8">
         <v>5.5</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E41" s="10">
         <v>45602</v>
       </c>
-      <c r="F41" s="4"/>
+      <c r="F41" s="10">
+        <v>45741</v>
+      </c>
       <c r="G41" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>134</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>67</v>
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I41" s="9"/>
       <c r="K41" s="8"/>
@@ -4504,24 +4503,26 @@
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C42" s="8">
         <v>5</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E42" s="10">
         <v>45602</v>
       </c>
-      <c r="F42" s="4"/>
+      <c r="F42" s="10">
+        <v>45741</v>
+      </c>
       <c r="G42" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>134</v>
-      </c>
-      <c r="H42" s="17" t="s">
-        <v>67</v>
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I42" s="9"/>
       <c r="K42" s="8"/>
@@ -4541,13 +4542,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C43" s="8">
         <v>5</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E43" s="10">
         <v>45602</v>
@@ -4582,13 +4583,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C44" s="8">
         <v>5</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E44" s="10">
         <v>45603</v>
@@ -4623,13 +4624,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C45" s="8">
         <v>5</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E45" s="10">
         <v>45603</v>
@@ -4664,13 +4665,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C46" s="8">
         <v>5</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E46" s="10">
         <v>45603</v>
@@ -4686,7 +4687,7 @@
         <v>30</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J46" s="4">
         <v>5.8</v>
@@ -4708,13 +4709,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C47" s="8">
         <v>5</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E47" s="10">
         <v>45603</v>
@@ -4749,13 +4750,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C48" s="8">
         <v>5</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E48" s="10">
         <v>45603</v>
@@ -4790,13 +4791,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C49" s="8">
         <v>5</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E49" s="10">
         <v>45603</v>
@@ -4831,13 +4832,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C50" s="8">
         <v>5</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E50" s="10">
         <v>45608</v>
@@ -4873,13 +4874,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C51" s="8">
         <v>5</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E51" s="10">
         <v>45608</v>
@@ -4915,13 +4916,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C52" s="8">
         <v>5</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E52" s="10">
         <v>45608</v>
@@ -4957,13 +4958,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C53" s="8">
         <v>6</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E53" s="10">
         <v>45608</v>
@@ -4979,7 +4980,7 @@
         <v>30</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J53" s="4">
         <v>5.9</v>
@@ -5001,13 +5002,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C54" s="8">
         <v>6</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E54" s="10">
         <v>45611</v>
@@ -5043,13 +5044,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C55" s="8">
         <v>6</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E55" s="10">
         <v>45611</v>
@@ -5085,13 +5086,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C56" s="8">
         <v>6</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E56" s="10">
         <v>45611</v>
@@ -5127,13 +5128,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C57" s="8">
         <v>6</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E57" s="10">
         <v>45612</v>
@@ -5169,13 +5170,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C58" s="8">
         <v>6</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E58" s="10">
         <v>45615</v>
@@ -5211,13 +5212,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C59" s="8">
         <v>6</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E59" s="10">
         <v>45615</v>
@@ -5253,13 +5254,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C60" s="8">
         <v>6</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E60" s="10">
         <v>45615</v>
@@ -5295,13 +5296,13 @@
         <v>59</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C61" s="8">
         <v>6</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E61" s="10">
         <v>45616</v>
@@ -5337,13 +5338,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C62" s="8">
         <v>6</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E62" s="10">
         <v>45617</v>
@@ -5379,13 +5380,13 @@
         <v>61</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C63" s="8">
         <v>6</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E63" s="10">
         <v>45617</v>
@@ -5421,13 +5422,13 @@
         <v>62</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C64" s="8">
         <v>5.5</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E64" s="10">
         <v>45632</v>
@@ -5460,13 +5461,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C65" s="8">
         <v>6</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E65" s="10">
         <v>45639</v>
@@ -5502,13 +5503,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C66" s="8">
         <v>6</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E66" s="10">
         <v>45643</v>
@@ -5544,13 +5545,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C67" s="8">
         <v>6</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E67" s="10">
         <v>45644</v>
@@ -5586,13 +5587,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C68" s="8">
         <v>6</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E68" s="10">
         <v>45644</v>
@@ -5628,13 +5629,13 @@
         <v>67</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C69" s="8">
         <v>6</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E69" s="10">
         <v>45645</v>
@@ -5670,13 +5671,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C70" s="8">
         <v>6</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E70" s="10">
         <v>45645</v>
@@ -5712,13 +5713,13 @@
         <v>69</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C71" s="8">
         <v>6</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E71" s="10">
         <v>45645</v>
@@ -5754,13 +5755,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C72" s="8">
         <v>7.5</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E72" s="10">
         <v>45680</v>
@@ -5796,27 +5797,29 @@
         <v>71</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C73" s="8">
         <v>7</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E73" s="10">
         <v>45707</v>
       </c>
-      <c r="F73" s="4"/>
+      <c r="F73" s="10">
+        <v>45741</v>
+      </c>
       <c r="G73" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="H73" s="8" t="s">
-        <v>167</v>
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="H73" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I73" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K73" s="8"/>
       <c r="L73" s="8"/>
@@ -5835,24 +5838,26 @@
         <v>72</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C74" s="8">
         <v>7</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E74" s="10">
         <v>45708</v>
       </c>
-      <c r="F74" s="4"/>
+      <c r="F74" s="10">
+        <v>45741</v>
+      </c>
       <c r="G74" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="H74" s="8" t="s">
-        <v>167</v>
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I74" s="9"/>
       <c r="K74" s="8"/>
@@ -5872,24 +5877,26 @@
         <v>73</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C75" s="8">
         <v>7</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E75" s="10">
         <v>45726</v>
       </c>
-      <c r="F75" s="4"/>
+      <c r="F75" s="10">
+        <v>45741</v>
+      </c>
       <c r="G75" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="H75" s="17" t="s">
-        <v>67</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="H75" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I75" s="9"/>
       <c r="J75" s="4">
@@ -5912,24 +5919,26 @@
         <v>74</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C76" s="8">
         <v>7</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E76" s="10">
         <v>45726</v>
       </c>
-      <c r="F76" s="4"/>
+      <c r="F76" s="10">
+        <v>45741</v>
+      </c>
       <c r="G76" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="H76" s="17" t="s">
-        <v>67</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="H76" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I76" s="9"/>
       <c r="J76" s="4">
@@ -5952,24 +5961,26 @@
         <v>75</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C77" s="8">
         <v>7</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E77" s="10">
         <v>45726</v>
       </c>
-      <c r="F77" s="4"/>
+      <c r="F77" s="10">
+        <v>45741</v>
+      </c>
       <c r="G77" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="H77" s="17" t="s">
-        <v>67</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="H77" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I77" s="9"/>
       <c r="J77" s="4">
@@ -5992,26 +6003,31 @@
         <v>76</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C78" s="8">
         <v>8</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E78" s="10">
         <v>45735</v>
       </c>
-      <c r="F78" s="4"/>
+      <c r="F78" s="10">
+        <v>45741</v>
+      </c>
       <c r="G78" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H78" s="8" t="s">
-        <v>167</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="H78" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I78" s="9"/>
+      <c r="J78" s="4">
+        <v>7.5</v>
+      </c>
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
@@ -6024,17 +6040,26 @@
       <c r="T78" s="8"/>
       <c r="U78" s="8"/>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>77</v>
       </c>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="E79" s="4"/>
+      <c r="B79" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C79" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E79" s="10">
+        <v>45740</v>
+      </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>1</v>
       </c>
       <c r="H79" s="8"/>
       <c r="I79" s="9"/>
@@ -6060,7 +6085,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H80" s="8"/>
       <c r="I80" s="9"/>
@@ -6086,7 +6111,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H81" s="8"/>
       <c r="I81" s="9"/>
@@ -6112,7 +6137,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H82" s="8"/>
       <c r="I82" s="9"/>
@@ -6138,7 +6163,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H83" s="8"/>
       <c r="I83" s="9"/>
@@ -6164,7 +6189,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H84" s="8"/>
       <c r="I84" s="9"/>
@@ -6190,7 +6215,7 @@
       <c r="F85" s="4"/>
       <c r="G85" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H85" s="8"/>
       <c r="I85" s="9"/>
@@ -6216,7 +6241,7 @@
       <c r="F86" s="4"/>
       <c r="G86" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H86" s="8"/>
       <c r="I86" s="9"/>
@@ -6242,7 +6267,7 @@
       <c r="F87" s="4"/>
       <c r="G87" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H87" s="8"/>
       <c r="I87" s="9"/>
@@ -6268,7 +6293,7 @@
       <c r="F88" s="4"/>
       <c r="G88" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H88" s="8"/>
       <c r="I88" s="9"/>
@@ -6294,7 +6319,7 @@
       <c r="F89" s="4"/>
       <c r="G89" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H89" s="8"/>
       <c r="I89" s="9"/>
@@ -6320,7 +6345,7 @@
       <c r="F90" s="4"/>
       <c r="G90" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H90" s="8"/>
       <c r="I90" s="9"/>
@@ -6346,7 +6371,7 @@
       <c r="F91" s="4"/>
       <c r="G91" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H91" s="8"/>
       <c r="I91" s="9"/>
@@ -6372,7 +6397,7 @@
       <c r="F92" s="4"/>
       <c r="G92" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H92" s="8"/>
       <c r="I92" s="9"/>
@@ -6398,7 +6423,7 @@
       <c r="F93" s="4"/>
       <c r="G93" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H93" s="8"/>
       <c r="I93" s="9"/>
@@ -6424,7 +6449,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H94" s="8"/>
       <c r="I94" s="9"/>
@@ -6450,7 +6475,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H95" s="8"/>
       <c r="I95" s="9"/>
@@ -6476,7 +6501,7 @@
       <c r="F96" s="4"/>
       <c r="G96" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H96" s="8"/>
       <c r="I96" s="9"/>
@@ -6502,7 +6527,7 @@
       <c r="F97" s="4"/>
       <c r="G97" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="9"/>
@@ -6528,7 +6553,7 @@
       <c r="F98" s="4"/>
       <c r="G98" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H98" s="8"/>
       <c r="I98" s="9"/>
@@ -6554,7 +6579,7 @@
       <c r="F99" s="4"/>
       <c r="G99" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H99" s="8"/>
       <c r="I99" s="9"/>
@@ -6580,7 +6605,7 @@
       <c r="F100" s="4"/>
       <c r="G100" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H100" s="8"/>
       <c r="I100" s="9"/>
@@ -6606,7 +6631,7 @@
       <c r="F101" s="4"/>
       <c r="G101" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H101" s="8"/>
       <c r="I101" s="9"/>
@@ -6632,7 +6657,7 @@
       <c r="F102" s="4"/>
       <c r="G102" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H102" s="8"/>
       <c r="I102" s="9"/>
@@ -6658,7 +6683,7 @@
       <c r="F103" s="4"/>
       <c r="G103" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H103" s="8"/>
       <c r="I103" s="9"/>
@@ -6684,7 +6709,7 @@
       <c r="F104" s="4"/>
       <c r="G104" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H104" s="8"/>
       <c r="I104" s="9"/>
@@ -6710,7 +6735,7 @@
       <c r="F105" s="4"/>
       <c r="G105" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H105" s="8"/>
       <c r="I105" s="9"/>
@@ -6736,7 +6761,7 @@
       <c r="F106" s="4"/>
       <c r="G106" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H106" s="8"/>
       <c r="I106" s="9"/>
@@ -6762,7 +6787,7 @@
       <c r="F107" s="4"/>
       <c r="G107" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H107" s="8"/>
       <c r="I107" s="9"/>
@@ -6788,7 +6813,7 @@
       <c r="F108" s="4"/>
       <c r="G108" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H108" s="8"/>
       <c r="I108" s="9"/>
@@ -6814,7 +6839,7 @@
       <c r="F109" s="4"/>
       <c r="G109" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H109" s="8"/>
       <c r="I109" s="9"/>
@@ -6840,7 +6865,7 @@
       <c r="F110" s="4"/>
       <c r="G110" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H110" s="8"/>
       <c r="I110" s="9"/>
@@ -6866,7 +6891,7 @@
       <c r="F111" s="4"/>
       <c r="G111" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H111" s="8"/>
       <c r="I111" s="9"/>
@@ -6892,7 +6917,7 @@
       <c r="F112" s="4"/>
       <c r="G112" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H112" s="8"/>
       <c r="I112" s="9"/>
@@ -6918,7 +6943,7 @@
       <c r="F113" s="4"/>
       <c r="G113" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H113" s="8"/>
       <c r="I113" s="9"/>
@@ -6944,7 +6969,7 @@
       <c r="F114" s="4"/>
       <c r="G114" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H114" s="8"/>
       <c r="I114" s="9"/>
@@ -6970,7 +6995,7 @@
       <c r="F115" s="4"/>
       <c r="G115" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H115" s="8"/>
       <c r="I115" s="9"/>
@@ -6996,7 +7021,7 @@
       <c r="F116" s="4"/>
       <c r="G116" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H116" s="8"/>
       <c r="I116" s="9"/>
@@ -7022,7 +7047,7 @@
       <c r="F117" s="4"/>
       <c r="G117" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H117" s="8"/>
       <c r="I117" s="9"/>
@@ -7048,7 +7073,7 @@
       <c r="F118" s="4"/>
       <c r="G118" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H118" s="8"/>
       <c r="I118" s="9"/>
@@ -7074,7 +7099,7 @@
       <c r="F119" s="4"/>
       <c r="G119" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H119" s="8"/>
       <c r="I119" s="9"/>
@@ -7100,7 +7125,7 @@
       <c r="F120" s="4"/>
       <c r="G120" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H120" s="8"/>
       <c r="I120" s="9"/>
@@ -7126,7 +7151,7 @@
       <c r="F121" s="4"/>
       <c r="G121" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H121" s="8"/>
       <c r="I121" s="9"/>
@@ -7152,7 +7177,7 @@
       <c r="F122" s="4"/>
       <c r="G122" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H122" s="8"/>
       <c r="I122" s="9"/>
@@ -7178,7 +7203,7 @@
       <c r="F123" s="4"/>
       <c r="G123" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H123" s="8"/>
       <c r="I123" s="9"/>
@@ -7204,7 +7229,7 @@
       <c r="F124" s="4"/>
       <c r="G124" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H124" s="8"/>
       <c r="I124" s="9"/>
@@ -7230,7 +7255,7 @@
       <c r="F125" s="4"/>
       <c r="G125" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H125" s="8"/>
       <c r="I125" s="9"/>
@@ -7256,7 +7281,7 @@
       <c r="F126" s="4"/>
       <c r="G126" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H126" s="8"/>
       <c r="I126" s="9"/>
@@ -7282,7 +7307,7 @@
       <c r="F127" s="4"/>
       <c r="G127" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H127" s="8"/>
       <c r="I127" s="9"/>
@@ -7308,7 +7333,7 @@
       <c r="F128" s="4"/>
       <c r="G128" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H128" s="8"/>
       <c r="I128" s="9"/>
@@ -7334,7 +7359,7 @@
       <c r="F129" s="4"/>
       <c r="G129" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H129" s="8"/>
       <c r="I129" s="9"/>
@@ -7360,7 +7385,7 @@
       <c r="F130" s="4"/>
       <c r="G130" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H130" s="8"/>
       <c r="I130" s="9"/>
@@ -7386,7 +7411,7 @@
       <c r="F131" s="4"/>
       <c r="G131" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="H131" s="8"/>
       <c r="I131" s="9"/>
@@ -8346,7 +8371,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8354,7 +8379,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -8362,7 +8387,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -8370,7 +8395,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -8378,7 +8403,7 @@
         <v>4.5</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -8386,7 +8411,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -8394,7 +8419,7 @@
         <v>5.5</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -8402,7 +8427,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -8410,7 +8435,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -8418,7 +8443,7 @@
         <v>7.5</v>
       </c>
       <c r="B11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -8426,7 +8451,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -8454,22 +8479,22 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
         <v>199</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>200</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>201</v>
       </c>
-      <c r="E2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F2" t="s">
-        <v>203</v>
-      </c>
       <c r="G2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8477,22 +8502,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8500,19 +8525,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>233</v>
+        <v>210</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>231</v>
       </c>
       <c r="G4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -8520,13 +8545,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>216</v>
+        <v>209</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>214</v>
       </c>
       <c r="G5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8534,13 +8559,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8548,13 +8573,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" t="s">
         <v>217</v>
       </c>
-      <c r="C7" t="s">
-        <v>219</v>
-      </c>
       <c r="G7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -8562,13 +8587,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -8576,21 +8601,21 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>226</v>
+      <c r="B10" s="17" t="s">
+        <v>224</v>
       </c>
       <c r="G10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -8598,10 +8623,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -8609,10 +8634,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>